<commit_message>
Added W-113 Diet and Lit
</commit_message>
<xml_diff>
--- a/Diets/Data/2018 Diets.xlsx
+++ b/Diets/Data/2018 Diets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Cedar/Google Drive/Thesis/Current Projects/Diets/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Cedar/Desktop/Thesis/Diets/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4164" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5049" uniqueCount="95">
   <si>
     <t>Coll. Date</t>
   </si>
@@ -298,6 +298,24 @@
   </si>
   <si>
     <t>TAT</t>
+  </si>
+  <si>
+    <t>W-113</t>
+  </si>
+  <si>
+    <t>Salamander</t>
+  </si>
+  <si>
+    <t>SImuliidae</t>
+  </si>
+  <si>
+    <t>DIxidae</t>
+  </si>
+  <si>
+    <t>DIptera</t>
+  </si>
+  <si>
+    <t>Amph</t>
   </si>
 </sst>
 </file>
@@ -613,11 +631,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L685"/>
+  <dimension ref="A1:L786"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O11" sqref="O11"/>
+      <pane ySplit="1" topLeftCell="A767" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A775" sqref="A775:L797"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21971,208 +21989,4667 @@
       </c>
     </row>
     <row r="635" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A635" s="1"/>
-      <c r="K635" s="1"/>
+      <c r="A635" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B635" t="s">
+        <v>89</v>
+      </c>
+      <c r="C635" t="s">
+        <v>75</v>
+      </c>
+      <c r="D635" t="s">
+        <v>8</v>
+      </c>
+      <c r="E635">
+        <v>1</v>
+      </c>
+      <c r="F635">
+        <v>10</v>
+      </c>
+      <c r="G635" t="s">
+        <v>26</v>
+      </c>
+      <c r="H635" t="s">
+        <v>31</v>
+      </c>
+      <c r="I635" t="s">
+        <v>49</v>
+      </c>
+      <c r="J635" t="s">
+        <v>18</v>
+      </c>
+      <c r="K635" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="636" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A636" s="1"/>
-      <c r="K636" s="1"/>
+      <c r="A636" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B636" t="s">
+        <v>89</v>
+      </c>
+      <c r="C636" t="s">
+        <v>75</v>
+      </c>
+      <c r="D636" t="s">
+        <v>8</v>
+      </c>
+      <c r="E636">
+        <v>1</v>
+      </c>
+      <c r="F636">
+        <v>10</v>
+      </c>
+      <c r="G636" t="s">
+        <v>26</v>
+      </c>
+      <c r="H636" t="s">
+        <v>31</v>
+      </c>
+      <c r="I636" t="s">
+        <v>49</v>
+      </c>
+      <c r="J636" t="s">
+        <v>18</v>
+      </c>
+      <c r="K636" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="637" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A637" s="1"/>
-      <c r="K637" s="1"/>
+      <c r="A637" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B637" t="s">
+        <v>89</v>
+      </c>
+      <c r="C637" t="s">
+        <v>75</v>
+      </c>
+      <c r="D637" t="s">
+        <v>8</v>
+      </c>
+      <c r="E637">
+        <v>1</v>
+      </c>
+      <c r="F637">
+        <v>10</v>
+      </c>
+      <c r="G637" t="s">
+        <v>26</v>
+      </c>
+      <c r="H637" t="s">
+        <v>19</v>
+      </c>
+      <c r="J637" t="s">
+        <v>18</v>
+      </c>
+      <c r="K637" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="638" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A638" s="1"/>
-      <c r="K638" s="1"/>
+      <c r="A638" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B638" t="s">
+        <v>89</v>
+      </c>
+      <c r="C638" t="s">
+        <v>75</v>
+      </c>
+      <c r="D638" t="s">
+        <v>8</v>
+      </c>
+      <c r="E638">
+        <v>1</v>
+      </c>
+      <c r="F638">
+        <v>10</v>
+      </c>
+      <c r="G638" t="s">
+        <v>26</v>
+      </c>
+      <c r="H638" t="s">
+        <v>53</v>
+      </c>
+      <c r="J638" t="s">
+        <v>17</v>
+      </c>
+      <c r="K638" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="639" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A639" s="1"/>
-      <c r="K639" s="1"/>
+      <c r="A639" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B639" t="s">
+        <v>89</v>
+      </c>
+      <c r="C639" t="s">
+        <v>75</v>
+      </c>
+      <c r="D639" t="s">
+        <v>8</v>
+      </c>
+      <c r="E639">
+        <v>1</v>
+      </c>
+      <c r="F639">
+        <v>10</v>
+      </c>
+      <c r="G639" t="s">
+        <v>26</v>
+      </c>
+      <c r="H639" t="s">
+        <v>19</v>
+      </c>
+      <c r="J639" t="s">
+        <v>18</v>
+      </c>
+      <c r="K639" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="640" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A640" s="1"/>
-      <c r="K640" s="1"/>
+      <c r="A640" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B640" t="s">
+        <v>89</v>
+      </c>
+      <c r="C640" t="s">
+        <v>75</v>
+      </c>
+      <c r="D640" t="s">
+        <v>8</v>
+      </c>
+      <c r="E640">
+        <v>1</v>
+      </c>
+      <c r="F640">
+        <v>10</v>
+      </c>
+      <c r="G640" t="s">
+        <v>26</v>
+      </c>
+      <c r="H640" t="s">
+        <v>44</v>
+      </c>
+      <c r="J640" t="s">
+        <v>17</v>
+      </c>
+      <c r="K640" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="641" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A641" s="1"/>
-      <c r="K641" s="1"/>
+      <c r="A641" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B641" t="s">
+        <v>89</v>
+      </c>
+      <c r="C641" t="s">
+        <v>75</v>
+      </c>
+      <c r="D641" t="s">
+        <v>8</v>
+      </c>
+      <c r="E641">
+        <v>1</v>
+      </c>
+      <c r="F641">
+        <v>10</v>
+      </c>
+      <c r="G641" t="s">
+        <v>26</v>
+      </c>
+      <c r="H641" t="s">
+        <v>21</v>
+      </c>
+      <c r="J641" t="s">
+        <v>18</v>
+      </c>
+      <c r="K641" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="642" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A642" s="1"/>
-      <c r="K642" s="1"/>
+      <c r="A642" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B642" t="s">
+        <v>89</v>
+      </c>
+      <c r="C642" t="s">
+        <v>75</v>
+      </c>
+      <c r="D642" t="s">
+        <v>8</v>
+      </c>
+      <c r="E642">
+        <v>1</v>
+      </c>
+      <c r="F642">
+        <v>10</v>
+      </c>
+      <c r="G642" t="s">
+        <v>26</v>
+      </c>
+      <c r="H642" t="s">
+        <v>19</v>
+      </c>
+      <c r="J642" t="s">
+        <v>17</v>
+      </c>
+      <c r="K642" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="643" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A643" s="1"/>
-      <c r="K643" s="1"/>
+      <c r="A643" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B643" t="s">
+        <v>89</v>
+      </c>
+      <c r="C643" t="s">
+        <v>75</v>
+      </c>
+      <c r="D643" t="s">
+        <v>8</v>
+      </c>
+      <c r="E643">
+        <v>1</v>
+      </c>
+      <c r="F643">
+        <v>10</v>
+      </c>
+      <c r="G643" t="s">
+        <v>26</v>
+      </c>
+      <c r="H643" t="s">
+        <v>19</v>
+      </c>
+      <c r="I643" t="s">
+        <v>42</v>
+      </c>
+      <c r="J643" t="s">
+        <v>13</v>
+      </c>
+      <c r="K643" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="644" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A644" s="1"/>
-      <c r="K644" s="1"/>
+      <c r="A644" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B644" t="s">
+        <v>89</v>
+      </c>
+      <c r="C644" t="s">
+        <v>75</v>
+      </c>
+      <c r="D644" t="s">
+        <v>8</v>
+      </c>
+      <c r="E644">
+        <v>1</v>
+      </c>
+      <c r="F644">
+        <v>10</v>
+      </c>
+      <c r="G644" t="s">
+        <v>26</v>
+      </c>
+      <c r="H644" t="s">
+        <v>54</v>
+      </c>
+      <c r="J644" t="s">
+        <v>17</v>
+      </c>
+      <c r="K644" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="645" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A645" s="1"/>
-      <c r="K645" s="1"/>
+      <c r="A645" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B645" t="s">
+        <v>89</v>
+      </c>
+      <c r="C645" t="s">
+        <v>75</v>
+      </c>
+      <c r="D645" t="s">
+        <v>8</v>
+      </c>
+      <c r="E645">
+        <v>1</v>
+      </c>
+      <c r="F645">
+        <v>10</v>
+      </c>
+      <c r="G645" t="s">
+        <v>26</v>
+      </c>
+      <c r="H645" t="s">
+        <v>19</v>
+      </c>
+      <c r="J645" t="s">
+        <v>17</v>
+      </c>
+      <c r="K645" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="646" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A646" s="1"/>
-      <c r="K646" s="1"/>
+      <c r="A646" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B646" t="s">
+        <v>89</v>
+      </c>
+      <c r="C646" t="s">
+        <v>75</v>
+      </c>
+      <c r="D646" t="s">
+        <v>8</v>
+      </c>
+      <c r="E646">
+        <v>1</v>
+      </c>
+      <c r="F646">
+        <v>10</v>
+      </c>
+      <c r="G646" t="s">
+        <v>26</v>
+      </c>
+      <c r="H646" t="s">
+        <v>19</v>
+      </c>
+      <c r="J646" t="s">
+        <v>17</v>
+      </c>
+      <c r="K646" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="647" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A647" s="1"/>
-      <c r="K647" s="1"/>
+      <c r="A647" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B647" t="s">
+        <v>89</v>
+      </c>
+      <c r="C647" t="s">
+        <v>75</v>
+      </c>
+      <c r="D647" t="s">
+        <v>8</v>
+      </c>
+      <c r="E647">
+        <v>1</v>
+      </c>
+      <c r="F647">
+        <v>6</v>
+      </c>
+      <c r="G647" t="s">
+        <v>26</v>
+      </c>
+      <c r="H647" t="s">
+        <v>20</v>
+      </c>
+      <c r="J647" t="s">
+        <v>17</v>
+      </c>
+      <c r="K647" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="648" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A648" s="1"/>
-      <c r="K648" s="1"/>
+      <c r="A648" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B648" t="s">
+        <v>89</v>
+      </c>
+      <c r="C648" t="s">
+        <v>75</v>
+      </c>
+      <c r="D648" t="s">
+        <v>8</v>
+      </c>
+      <c r="E648">
+        <v>1</v>
+      </c>
+      <c r="F648">
+        <v>6</v>
+      </c>
+      <c r="G648" t="s">
+        <v>24</v>
+      </c>
+      <c r="H648" t="s">
+        <v>21</v>
+      </c>
+      <c r="J648" t="s">
+        <v>18</v>
+      </c>
+      <c r="K648" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="649" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A649" s="1"/>
-      <c r="K649" s="1"/>
+      <c r="A649" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B649" t="s">
+        <v>89</v>
+      </c>
+      <c r="C649" t="s">
+        <v>75</v>
+      </c>
+      <c r="D649" t="s">
+        <v>8</v>
+      </c>
+      <c r="E649">
+        <v>1</v>
+      </c>
+      <c r="F649">
+        <v>6</v>
+      </c>
+      <c r="G649" t="s">
+        <v>26</v>
+      </c>
+      <c r="H649" t="s">
+        <v>19</v>
+      </c>
+      <c r="J649" t="s">
+        <v>18</v>
+      </c>
+      <c r="K649" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="650" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A650" s="1"/>
-      <c r="K650" s="1"/>
+      <c r="A650" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B650" t="s">
+        <v>89</v>
+      </c>
+      <c r="C650" t="s">
+        <v>75</v>
+      </c>
+      <c r="D650" t="s">
+        <v>8</v>
+      </c>
+      <c r="E650">
+        <v>1</v>
+      </c>
+      <c r="F650">
+        <v>6</v>
+      </c>
+      <c r="G650" t="s">
+        <v>26</v>
+      </c>
+      <c r="H650" t="s">
+        <v>19</v>
+      </c>
+      <c r="J650" t="s">
+        <v>18</v>
+      </c>
+      <c r="K650" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="651" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A651" s="1"/>
-      <c r="K651" s="1"/>
+      <c r="A651" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B651" t="s">
+        <v>89</v>
+      </c>
+      <c r="C651" t="s">
+        <v>75</v>
+      </c>
+      <c r="D651" t="s">
+        <v>8</v>
+      </c>
+      <c r="E651">
+        <v>1</v>
+      </c>
+      <c r="F651">
+        <v>6</v>
+      </c>
+      <c r="G651" t="s">
+        <v>26</v>
+      </c>
+      <c r="H651" t="s">
+        <v>19</v>
+      </c>
+      <c r="J651" t="s">
+        <v>17</v>
+      </c>
+      <c r="K651" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="652" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A652" s="1"/>
-      <c r="K652" s="1"/>
+      <c r="A652" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B652" t="s">
+        <v>89</v>
+      </c>
+      <c r="C652" t="s">
+        <v>75</v>
+      </c>
+      <c r="D652" t="s">
+        <v>8</v>
+      </c>
+      <c r="E652">
+        <v>1</v>
+      </c>
+      <c r="F652">
+        <v>6</v>
+      </c>
+      <c r="G652" t="s">
+        <v>26</v>
+      </c>
+      <c r="H652" t="s">
+        <v>19</v>
+      </c>
+      <c r="I652" t="s">
+        <v>46</v>
+      </c>
+      <c r="J652" t="s">
+        <v>18</v>
+      </c>
+      <c r="K652" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="653" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A653" s="1"/>
-      <c r="K653" s="1"/>
+      <c r="A653" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B653" t="s">
+        <v>89</v>
+      </c>
+      <c r="C653" t="s">
+        <v>75</v>
+      </c>
+      <c r="D653" t="s">
+        <v>8</v>
+      </c>
+      <c r="E653">
+        <v>1</v>
+      </c>
+      <c r="F653">
+        <v>6</v>
+      </c>
+      <c r="G653" t="s">
+        <v>26</v>
+      </c>
+      <c r="H653" t="s">
+        <v>19</v>
+      </c>
+      <c r="J653" t="s">
+        <v>18</v>
+      </c>
+      <c r="K653" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="654" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A654" s="1"/>
-      <c r="K654" s="1"/>
+      <c r="A654" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B654" t="s">
+        <v>89</v>
+      </c>
+      <c r="C654" t="s">
+        <v>75</v>
+      </c>
+      <c r="D654" t="s">
+        <v>8</v>
+      </c>
+      <c r="E654">
+        <v>1</v>
+      </c>
+      <c r="F654">
+        <v>6</v>
+      </c>
+      <c r="G654" t="s">
+        <v>26</v>
+      </c>
+      <c r="H654" t="s">
+        <v>19</v>
+      </c>
+      <c r="J654" t="s">
+        <v>18</v>
+      </c>
+      <c r="K654" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="655" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A655" s="1"/>
-      <c r="K655" s="1"/>
+      <c r="A655" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B655" t="s">
+        <v>89</v>
+      </c>
+      <c r="C655" t="s">
+        <v>75</v>
+      </c>
+      <c r="D655" t="s">
+        <v>8</v>
+      </c>
+      <c r="E655">
+        <v>1</v>
+      </c>
+      <c r="F655">
+        <v>6</v>
+      </c>
+      <c r="G655" t="s">
+        <v>26</v>
+      </c>
+      <c r="H655" t="s">
+        <v>19</v>
+      </c>
+      <c r="J655" t="s">
+        <v>18</v>
+      </c>
+      <c r="K655" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="656" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A656" s="1"/>
-      <c r="K656" s="1"/>
+      <c r="A656" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B656" t="s">
+        <v>89</v>
+      </c>
+      <c r="C656" t="s">
+        <v>75</v>
+      </c>
+      <c r="D656" t="s">
+        <v>8</v>
+      </c>
+      <c r="E656">
+        <v>1</v>
+      </c>
+      <c r="F656">
+        <v>6</v>
+      </c>
+      <c r="G656" t="s">
+        <v>26</v>
+      </c>
+      <c r="H656" t="s">
+        <v>19</v>
+      </c>
+      <c r="J656" t="s">
+        <v>18</v>
+      </c>
+      <c r="K656" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="657" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A657" s="1"/>
-      <c r="K657" s="1"/>
+      <c r="A657" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B657" t="s">
+        <v>89</v>
+      </c>
+      <c r="C657" t="s">
+        <v>75</v>
+      </c>
+      <c r="D657" t="s">
+        <v>8</v>
+      </c>
+      <c r="E657">
+        <v>1</v>
+      </c>
+      <c r="F657">
+        <v>6</v>
+      </c>
+      <c r="G657" t="s">
+        <v>26</v>
+      </c>
+      <c r="H657" t="s">
+        <v>19</v>
+      </c>
+      <c r="J657" t="s">
+        <v>18</v>
+      </c>
+      <c r="K657" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="658" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A658" s="1"/>
-      <c r="K658" s="1"/>
+      <c r="A658" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B658" t="s">
+        <v>89</v>
+      </c>
+      <c r="C658" t="s">
+        <v>75</v>
+      </c>
+      <c r="D658" t="s">
+        <v>8</v>
+      </c>
+      <c r="E658">
+        <v>1</v>
+      </c>
+      <c r="F658">
+        <v>6</v>
+      </c>
+      <c r="G658" t="s">
+        <v>26</v>
+      </c>
+      <c r="H658" t="s">
+        <v>19</v>
+      </c>
+      <c r="J658" t="s">
+        <v>18</v>
+      </c>
+      <c r="K658" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="659" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A659" s="1"/>
-      <c r="K659" s="1"/>
+      <c r="A659" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B659" t="s">
+        <v>89</v>
+      </c>
+      <c r="C659" t="s">
+        <v>75</v>
+      </c>
+      <c r="D659" t="s">
+        <v>8</v>
+      </c>
+      <c r="E659">
+        <v>1</v>
+      </c>
+      <c r="F659">
+        <v>6</v>
+      </c>
+      <c r="G659" t="s">
+        <v>26</v>
+      </c>
+      <c r="H659" t="s">
+        <v>19</v>
+      </c>
+      <c r="J659" t="s">
+        <v>18</v>
+      </c>
+      <c r="K659" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="660" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A660" s="1"/>
-      <c r="K660" s="1"/>
+      <c r="A660" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B660" t="s">
+        <v>89</v>
+      </c>
+      <c r="C660" t="s">
+        <v>75</v>
+      </c>
+      <c r="D660" t="s">
+        <v>8</v>
+      </c>
+      <c r="E660">
+        <v>1</v>
+      </c>
+      <c r="F660">
+        <v>6</v>
+      </c>
+      <c r="G660" t="s">
+        <v>26</v>
+      </c>
+      <c r="H660" t="s">
+        <v>44</v>
+      </c>
+      <c r="J660" t="s">
+        <v>17</v>
+      </c>
+      <c r="K660" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="661" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A661" s="1"/>
-      <c r="K661" s="1"/>
+      <c r="A661" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B661" t="s">
+        <v>89</v>
+      </c>
+      <c r="C661" t="s">
+        <v>75</v>
+      </c>
+      <c r="D661" t="s">
+        <v>8</v>
+      </c>
+      <c r="E661">
+        <v>1</v>
+      </c>
+      <c r="F661">
+        <v>6</v>
+      </c>
+      <c r="G661" t="s">
+        <v>26</v>
+      </c>
+      <c r="H661" t="s">
+        <v>19</v>
+      </c>
+      <c r="J661" t="s">
+        <v>17</v>
+      </c>
+      <c r="K661" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="662" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A662" s="1"/>
-      <c r="K662" s="1"/>
+      <c r="A662" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B662" t="s">
+        <v>89</v>
+      </c>
+      <c r="C662" t="s">
+        <v>75</v>
+      </c>
+      <c r="D662" t="s">
+        <v>8</v>
+      </c>
+      <c r="E662">
+        <v>1</v>
+      </c>
+      <c r="F662">
+        <v>6</v>
+      </c>
+      <c r="G662" t="s">
+        <v>26</v>
+      </c>
+      <c r="H662" t="s">
+        <v>19</v>
+      </c>
+      <c r="J662" t="s">
+        <v>18</v>
+      </c>
+      <c r="K662" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="663" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A663" s="1"/>
-      <c r="K663" s="1"/>
+      <c r="A663" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B663" t="s">
+        <v>89</v>
+      </c>
+      <c r="C663" t="s">
+        <v>75</v>
+      </c>
+      <c r="D663" t="s">
+        <v>8</v>
+      </c>
+      <c r="E663">
+        <v>1</v>
+      </c>
+      <c r="F663">
+        <v>6</v>
+      </c>
+      <c r="G663" t="s">
+        <v>26</v>
+      </c>
+      <c r="H663" t="s">
+        <v>19</v>
+      </c>
+      <c r="I663" t="s">
+        <v>46</v>
+      </c>
+      <c r="J663" t="s">
+        <v>18</v>
+      </c>
+      <c r="K663" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="664" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A664" s="1"/>
-      <c r="K664" s="1"/>
+      <c r="A664" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B664" t="s">
+        <v>89</v>
+      </c>
+      <c r="C664" t="s">
+        <v>75</v>
+      </c>
+      <c r="D664" t="s">
+        <v>8</v>
+      </c>
+      <c r="E664">
+        <v>1</v>
+      </c>
+      <c r="F664">
+        <v>6</v>
+      </c>
+      <c r="G664" t="s">
+        <v>26</v>
+      </c>
+      <c r="H664" t="s">
+        <v>19</v>
+      </c>
+      <c r="I664" t="s">
+        <v>46</v>
+      </c>
+      <c r="J664" t="s">
+        <v>18</v>
+      </c>
+      <c r="K664" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="665" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A665" s="1"/>
-      <c r="K665" s="1"/>
+      <c r="A665" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B665" t="s">
+        <v>89</v>
+      </c>
+      <c r="C665" t="s">
+        <v>75</v>
+      </c>
+      <c r="D665" t="s">
+        <v>8</v>
+      </c>
+      <c r="E665">
+        <v>1</v>
+      </c>
+      <c r="F665">
+        <v>9</v>
+      </c>
+      <c r="G665" t="s">
+        <v>26</v>
+      </c>
+      <c r="H665" t="s">
+        <v>21</v>
+      </c>
+      <c r="I665" t="s">
+        <v>41</v>
+      </c>
+      <c r="J665" t="s">
+        <v>18</v>
+      </c>
+      <c r="K665" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="666" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A666" s="1"/>
-      <c r="K666" s="1"/>
+      <c r="A666" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B666" t="s">
+        <v>89</v>
+      </c>
+      <c r="C666" t="s">
+        <v>75</v>
+      </c>
+      <c r="D666" t="s">
+        <v>8</v>
+      </c>
+      <c r="E666">
+        <v>1</v>
+      </c>
+      <c r="F666">
+        <v>9</v>
+      </c>
+      <c r="G666" t="s">
+        <v>22</v>
+      </c>
+      <c r="H666" t="s">
+        <v>21</v>
+      </c>
+      <c r="I666" t="s">
+        <v>41</v>
+      </c>
+      <c r="J666" t="s">
+        <v>13</v>
+      </c>
+      <c r="K666" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="667" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A667" s="1"/>
-      <c r="K667" s="1"/>
+      <c r="A667" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B667" t="s">
+        <v>89</v>
+      </c>
+      <c r="C667" t="s">
+        <v>75</v>
+      </c>
+      <c r="D667" t="s">
+        <v>8</v>
+      </c>
+      <c r="E667">
+        <v>1</v>
+      </c>
+      <c r="F667">
+        <v>9</v>
+      </c>
+      <c r="G667" t="s">
+        <v>26</v>
+      </c>
+      <c r="H667" t="s">
+        <v>21</v>
+      </c>
+      <c r="I667" t="s">
+        <v>70</v>
+      </c>
+      <c r="J667" t="s">
+        <v>13</v>
+      </c>
+      <c r="K667" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="668" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A668" s="1"/>
-      <c r="K668" s="1"/>
+      <c r="A668" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B668" t="s">
+        <v>89</v>
+      </c>
+      <c r="C668" t="s">
+        <v>75</v>
+      </c>
+      <c r="D668" t="s">
+        <v>8</v>
+      </c>
+      <c r="E668">
+        <v>1</v>
+      </c>
+      <c r="F668">
+        <v>9</v>
+      </c>
+      <c r="G668" t="s">
+        <v>26</v>
+      </c>
+      <c r="H668" t="s">
+        <v>21</v>
+      </c>
+      <c r="J668" t="s">
+        <v>18</v>
+      </c>
+      <c r="K668" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="669" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A669" s="1"/>
-      <c r="K669" s="1"/>
+      <c r="A669" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B669" t="s">
+        <v>89</v>
+      </c>
+      <c r="C669" t="s">
+        <v>75</v>
+      </c>
+      <c r="D669" t="s">
+        <v>8</v>
+      </c>
+      <c r="E669">
+        <v>1</v>
+      </c>
+      <c r="F669">
+        <v>9</v>
+      </c>
+      <c r="G669" t="s">
+        <v>26</v>
+      </c>
+      <c r="H669" t="s">
+        <v>19</v>
+      </c>
+      <c r="J669" t="s">
+        <v>18</v>
+      </c>
+      <c r="K669" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="670" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A670" s="1"/>
-      <c r="K670" s="1"/>
+      <c r="A670" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B670" t="s">
+        <v>89</v>
+      </c>
+      <c r="C670" t="s">
+        <v>75</v>
+      </c>
+      <c r="D670" t="s">
+        <v>8</v>
+      </c>
+      <c r="E670">
+        <v>1</v>
+      </c>
+      <c r="F670">
+        <v>9</v>
+      </c>
+      <c r="G670" t="s">
+        <v>26</v>
+      </c>
+      <c r="H670" t="s">
+        <v>19</v>
+      </c>
+      <c r="I670" t="s">
+        <v>46</v>
+      </c>
+      <c r="J670" t="s">
+        <v>13</v>
+      </c>
+      <c r="K670" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="671" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A671" s="1"/>
-      <c r="K671" s="1"/>
+      <c r="A671" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B671" t="s">
+        <v>89</v>
+      </c>
+      <c r="C671" t="s">
+        <v>75</v>
+      </c>
+      <c r="D671" t="s">
+        <v>8</v>
+      </c>
+      <c r="E671">
+        <v>1</v>
+      </c>
+      <c r="F671">
+        <v>3</v>
+      </c>
+      <c r="G671" t="s">
+        <v>26</v>
+      </c>
+      <c r="H671" t="s">
+        <v>90</v>
+      </c>
+      <c r="J671" t="s">
+        <v>13</v>
+      </c>
+      <c r="K671" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="672" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A672" s="1"/>
-      <c r="K672" s="1"/>
+      <c r="A672" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B672" t="s">
+        <v>89</v>
+      </c>
+      <c r="C672" t="s">
+        <v>75</v>
+      </c>
+      <c r="D672" t="s">
+        <v>8</v>
+      </c>
+      <c r="E672">
+        <v>1</v>
+      </c>
+      <c r="F672">
+        <v>3</v>
+      </c>
+      <c r="G672" t="s">
+        <v>26</v>
+      </c>
+      <c r="H672" t="s">
+        <v>25</v>
+      </c>
+      <c r="I672" t="s">
+        <v>29</v>
+      </c>
+      <c r="J672" t="s">
+        <v>13</v>
+      </c>
+      <c r="K672" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="673" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A673" s="1"/>
-      <c r="K673" s="1"/>
+      <c r="A673" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B673" t="s">
+        <v>89</v>
+      </c>
+      <c r="C673" t="s">
+        <v>75</v>
+      </c>
+      <c r="D673" t="s">
+        <v>8</v>
+      </c>
+      <c r="E673">
+        <v>1</v>
+      </c>
+      <c r="F673">
+        <v>3</v>
+      </c>
+      <c r="G673" t="s">
+        <v>26</v>
+      </c>
+      <c r="H673" t="s">
+        <v>25</v>
+      </c>
+      <c r="I673" t="s">
+        <v>29</v>
+      </c>
+      <c r="J673" t="s">
+        <v>13</v>
+      </c>
+      <c r="K673" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="674" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A674" s="1"/>
-      <c r="K674" s="1"/>
+      <c r="A674" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B674" t="s">
+        <v>89</v>
+      </c>
+      <c r="C674" t="s">
+        <v>75</v>
+      </c>
+      <c r="D674" t="s">
+        <v>8</v>
+      </c>
+      <c r="E674">
+        <v>1</v>
+      </c>
+      <c r="F674">
+        <v>3</v>
+      </c>
+      <c r="G674" t="s">
+        <v>26</v>
+      </c>
+      <c r="H674" t="s">
+        <v>25</v>
+      </c>
+      <c r="I674" t="s">
+        <v>59</v>
+      </c>
+      <c r="J674" t="s">
+        <v>13</v>
+      </c>
+      <c r="K674" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="675" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A675" s="1"/>
-      <c r="K675" s="1"/>
+      <c r="A675" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B675" t="s">
+        <v>89</v>
+      </c>
+      <c r="C675" t="s">
+        <v>75</v>
+      </c>
+      <c r="D675" t="s">
+        <v>8</v>
+      </c>
+      <c r="E675">
+        <v>1</v>
+      </c>
+      <c r="F675">
+        <v>3</v>
+      </c>
+      <c r="G675" t="s">
+        <v>26</v>
+      </c>
+      <c r="H675" t="s">
+        <v>45</v>
+      </c>
+      <c r="J675" t="s">
+        <v>13</v>
+      </c>
+      <c r="K675" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="676" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A676" s="1"/>
-      <c r="K676" s="1"/>
+      <c r="A676" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B676" t="s">
+        <v>89</v>
+      </c>
+      <c r="C676" t="s">
+        <v>75</v>
+      </c>
+      <c r="D676" t="s">
+        <v>8</v>
+      </c>
+      <c r="E676">
+        <v>1</v>
+      </c>
+      <c r="F676">
+        <v>3</v>
+      </c>
+      <c r="G676" t="s">
+        <v>26</v>
+      </c>
+      <c r="H676" t="s">
+        <v>45</v>
+      </c>
+      <c r="J676" t="s">
+        <v>13</v>
+      </c>
+      <c r="K676" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="677" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A677" s="1"/>
-      <c r="K677" s="1"/>
+      <c r="A677" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B677" t="s">
+        <v>89</v>
+      </c>
+      <c r="C677" t="s">
+        <v>75</v>
+      </c>
+      <c r="D677" t="s">
+        <v>8</v>
+      </c>
+      <c r="E677">
+        <v>1</v>
+      </c>
+      <c r="F677">
+        <v>3</v>
+      </c>
+      <c r="G677" t="s">
+        <v>26</v>
+      </c>
+      <c r="H677" t="s">
+        <v>54</v>
+      </c>
+      <c r="J677" t="s">
+        <v>17</v>
+      </c>
+      <c r="K677" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="678" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A678" s="1"/>
-      <c r="K678" s="1"/>
+      <c r="A678" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B678" t="s">
+        <v>89</v>
+      </c>
+      <c r="C678" t="s">
+        <v>75</v>
+      </c>
+      <c r="D678" t="s">
+        <v>8</v>
+      </c>
+      <c r="E678">
+        <v>1</v>
+      </c>
+      <c r="F678">
+        <v>3</v>
+      </c>
+      <c r="G678" t="s">
+        <v>26</v>
+      </c>
+      <c r="H678" t="s">
+        <v>44</v>
+      </c>
+      <c r="J678" t="s">
+        <v>17</v>
+      </c>
+      <c r="K678" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="679" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A679" s="1"/>
-      <c r="K679" s="1"/>
+      <c r="A679" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B679" t="s">
+        <v>89</v>
+      </c>
+      <c r="C679" t="s">
+        <v>75</v>
+      </c>
+      <c r="D679" t="s">
+        <v>8</v>
+      </c>
+      <c r="E679">
+        <v>1</v>
+      </c>
+      <c r="F679">
+        <v>3</v>
+      </c>
+      <c r="G679" t="s">
+        <v>26</v>
+      </c>
+      <c r="H679" t="s">
+        <v>34</v>
+      </c>
+      <c r="I679" t="s">
+        <v>64</v>
+      </c>
+      <c r="J679" t="s">
+        <v>18</v>
+      </c>
+      <c r="K679" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="680" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A680" s="1"/>
-      <c r="K680" s="1"/>
+      <c r="A680" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B680" t="s">
+        <v>89</v>
+      </c>
+      <c r="C680" t="s">
+        <v>75</v>
+      </c>
+      <c r="D680" t="s">
+        <v>8</v>
+      </c>
+      <c r="E680">
+        <v>1</v>
+      </c>
+      <c r="F680">
+        <v>3</v>
+      </c>
+      <c r="G680" t="s">
+        <v>24</v>
+      </c>
+      <c r="H680" t="s">
+        <v>21</v>
+      </c>
+      <c r="J680" t="s">
+        <v>13</v>
+      </c>
+      <c r="K680" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="681" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A681" s="1"/>
-      <c r="K681" s="1"/>
+      <c r="A681" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B681" t="s">
+        <v>89</v>
+      </c>
+      <c r="C681" t="s">
+        <v>75</v>
+      </c>
+      <c r="D681" t="s">
+        <v>8</v>
+      </c>
+      <c r="E681">
+        <v>1</v>
+      </c>
+      <c r="F681">
+        <v>3</v>
+      </c>
+      <c r="G681" t="s">
+        <v>24</v>
+      </c>
+      <c r="H681" t="s">
+        <v>21</v>
+      </c>
+      <c r="J681" t="s">
+        <v>13</v>
+      </c>
+      <c r="K681" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="682" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A682" s="1"/>
-      <c r="K682" s="1"/>
+      <c r="A682" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B682" t="s">
+        <v>89</v>
+      </c>
+      <c r="C682" t="s">
+        <v>75</v>
+      </c>
+      <c r="D682" t="s">
+        <v>8</v>
+      </c>
+      <c r="E682">
+        <v>1</v>
+      </c>
+      <c r="F682">
+        <v>3</v>
+      </c>
+      <c r="G682" t="s">
+        <v>26</v>
+      </c>
+      <c r="H682" t="s">
+        <v>20</v>
+      </c>
+      <c r="J682" t="s">
+        <v>17</v>
+      </c>
+      <c r="K682" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="683" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A683" s="1"/>
-      <c r="K683" s="1"/>
+      <c r="A683" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B683" t="s">
+        <v>89</v>
+      </c>
+      <c r="C683" t="s">
+        <v>75</v>
+      </c>
+      <c r="D683" t="s">
+        <v>8</v>
+      </c>
+      <c r="E683">
+        <v>1</v>
+      </c>
+      <c r="F683">
+        <v>3</v>
+      </c>
+      <c r="G683" t="s">
+        <v>22</v>
+      </c>
+      <c r="H683" t="s">
+        <v>31</v>
+      </c>
+      <c r="J683" t="s">
+        <v>13</v>
+      </c>
+      <c r="K683" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="684" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A684" s="1"/>
-      <c r="K684" s="1"/>
+      <c r="A684" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B684" t="s">
+        <v>89</v>
+      </c>
+      <c r="C684" t="s">
+        <v>75</v>
+      </c>
+      <c r="D684" t="s">
+        <v>8</v>
+      </c>
+      <c r="E684">
+        <v>1</v>
+      </c>
+      <c r="F684">
+        <v>3</v>
+      </c>
+      <c r="G684" t="s">
+        <v>26</v>
+      </c>
+      <c r="H684" t="s">
+        <v>34</v>
+      </c>
+      <c r="I684" t="s">
+        <v>64</v>
+      </c>
+      <c r="J684" t="s">
+        <v>18</v>
+      </c>
+      <c r="K684" s="1">
+        <v>43493</v>
+      </c>
     </row>
     <row r="685" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A685" s="1"/>
-      <c r="K685" s="1"/>
+      <c r="A685" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B685" t="s">
+        <v>89</v>
+      </c>
+      <c r="C685" t="s">
+        <v>75</v>
+      </c>
+      <c r="D685" t="s">
+        <v>8</v>
+      </c>
+      <c r="E685">
+        <v>1</v>
+      </c>
+      <c r="F685">
+        <v>3</v>
+      </c>
+      <c r="G685" t="s">
+        <v>24</v>
+      </c>
+      <c r="H685" t="s">
+        <v>21</v>
+      </c>
+      <c r="J685" t="s">
+        <v>13</v>
+      </c>
+      <c r="K685" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="686" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A686" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B686" t="s">
+        <v>89</v>
+      </c>
+      <c r="C686" t="s">
+        <v>75</v>
+      </c>
+      <c r="D686" t="s">
+        <v>8</v>
+      </c>
+      <c r="E686">
+        <v>1</v>
+      </c>
+      <c r="F686">
+        <v>5</v>
+      </c>
+      <c r="G686" t="s">
+        <v>26</v>
+      </c>
+      <c r="H686" t="s">
+        <v>54</v>
+      </c>
+      <c r="J686" t="s">
+        <v>17</v>
+      </c>
+      <c r="K686" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="687" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A687" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B687" t="s">
+        <v>89</v>
+      </c>
+      <c r="C687" t="s">
+        <v>75</v>
+      </c>
+      <c r="D687" t="s">
+        <v>8</v>
+      </c>
+      <c r="E687">
+        <v>1</v>
+      </c>
+      <c r="F687">
+        <v>5</v>
+      </c>
+      <c r="G687" t="s">
+        <v>26</v>
+      </c>
+      <c r="H687" t="s">
+        <v>19</v>
+      </c>
+      <c r="J687" t="s">
+        <v>17</v>
+      </c>
+      <c r="K687" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="688" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A688" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B688" t="s">
+        <v>89</v>
+      </c>
+      <c r="C688" t="s">
+        <v>75</v>
+      </c>
+      <c r="D688" t="s">
+        <v>8</v>
+      </c>
+      <c r="E688">
+        <v>1</v>
+      </c>
+      <c r="F688">
+        <v>5</v>
+      </c>
+      <c r="G688" t="s">
+        <v>24</v>
+      </c>
+      <c r="H688" t="s">
+        <v>20</v>
+      </c>
+      <c r="J688" t="s">
+        <v>17</v>
+      </c>
+      <c r="K688" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="689" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A689" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B689" t="s">
+        <v>89</v>
+      </c>
+      <c r="C689" t="s">
+        <v>75</v>
+      </c>
+      <c r="D689" t="s">
+        <v>8</v>
+      </c>
+      <c r="E689">
+        <v>1</v>
+      </c>
+      <c r="F689">
+        <v>5</v>
+      </c>
+      <c r="G689" t="s">
+        <v>26</v>
+      </c>
+      <c r="H689" t="s">
+        <v>78</v>
+      </c>
+      <c r="J689" t="s">
+        <v>17</v>
+      </c>
+      <c r="K689" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="690" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A690" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B690" t="s">
+        <v>89</v>
+      </c>
+      <c r="C690" t="s">
+        <v>75</v>
+      </c>
+      <c r="D690" t="s">
+        <v>8</v>
+      </c>
+      <c r="E690">
+        <v>1</v>
+      </c>
+      <c r="F690">
+        <v>5</v>
+      </c>
+      <c r="G690" t="s">
+        <v>26</v>
+      </c>
+      <c r="H690" t="s">
+        <v>19</v>
+      </c>
+      <c r="I690" t="s">
+        <v>91</v>
+      </c>
+      <c r="J690" t="s">
+        <v>17</v>
+      </c>
+      <c r="K690" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="691" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A691" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B691" t="s">
+        <v>89</v>
+      </c>
+      <c r="C691" t="s">
+        <v>75</v>
+      </c>
+      <c r="D691" t="s">
+        <v>8</v>
+      </c>
+      <c r="E691">
+        <v>1</v>
+      </c>
+      <c r="F691">
+        <v>5</v>
+      </c>
+      <c r="G691" t="s">
+        <v>26</v>
+      </c>
+      <c r="H691" t="s">
+        <v>54</v>
+      </c>
+      <c r="J691" t="s">
+        <v>17</v>
+      </c>
+      <c r="K691" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="692" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A692" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B692" t="s">
+        <v>89</v>
+      </c>
+      <c r="C692" t="s">
+        <v>75</v>
+      </c>
+      <c r="D692" t="s">
+        <v>8</v>
+      </c>
+      <c r="E692">
+        <v>1</v>
+      </c>
+      <c r="F692">
+        <v>5</v>
+      </c>
+      <c r="G692" t="s">
+        <v>22</v>
+      </c>
+      <c r="H692" t="s">
+        <v>21</v>
+      </c>
+      <c r="J692" t="s">
+        <v>18</v>
+      </c>
+      <c r="K692" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="693" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A693" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B693" t="s">
+        <v>89</v>
+      </c>
+      <c r="C693" t="s">
+        <v>75</v>
+      </c>
+      <c r="D693" t="s">
+        <v>8</v>
+      </c>
+      <c r="E693">
+        <v>1</v>
+      </c>
+      <c r="F693">
+        <v>5</v>
+      </c>
+      <c r="G693" t="s">
+        <v>22</v>
+      </c>
+      <c r="H693" t="s">
+        <v>21</v>
+      </c>
+      <c r="J693" t="s">
+        <v>18</v>
+      </c>
+      <c r="K693" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="694" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A694" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B694" t="s">
+        <v>89</v>
+      </c>
+      <c r="C694" t="s">
+        <v>75</v>
+      </c>
+      <c r="D694" t="s">
+        <v>8</v>
+      </c>
+      <c r="E694">
+        <v>1</v>
+      </c>
+      <c r="F694">
+        <v>5</v>
+      </c>
+      <c r="G694" t="s">
+        <v>24</v>
+      </c>
+      <c r="H694" t="s">
+        <v>20</v>
+      </c>
+      <c r="J694" t="s">
+        <v>17</v>
+      </c>
+      <c r="K694" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="695" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A695" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B695" t="s">
+        <v>89</v>
+      </c>
+      <c r="C695" t="s">
+        <v>75</v>
+      </c>
+      <c r="D695" t="s">
+        <v>8</v>
+      </c>
+      <c r="E695">
+        <v>1</v>
+      </c>
+      <c r="F695">
+        <v>5</v>
+      </c>
+      <c r="G695" t="s">
+        <v>26</v>
+      </c>
+      <c r="H695" t="s">
+        <v>34</v>
+      </c>
+      <c r="I695" t="s">
+        <v>64</v>
+      </c>
+      <c r="J695" t="s">
+        <v>18</v>
+      </c>
+      <c r="K695" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="696" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A696" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B696" t="s">
+        <v>89</v>
+      </c>
+      <c r="C696" t="s">
+        <v>75</v>
+      </c>
+      <c r="D696" t="s">
+        <v>8</v>
+      </c>
+      <c r="E696">
+        <v>1</v>
+      </c>
+      <c r="F696">
+        <v>4</v>
+      </c>
+      <c r="G696" t="s">
+        <v>26</v>
+      </c>
+      <c r="H696" t="s">
+        <v>21</v>
+      </c>
+      <c r="J696" t="s">
+        <v>18</v>
+      </c>
+      <c r="K696" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="697" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A697" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B697" t="s">
+        <v>89</v>
+      </c>
+      <c r="C697" t="s">
+        <v>75</v>
+      </c>
+      <c r="D697" t="s">
+        <v>8</v>
+      </c>
+      <c r="E697">
+        <v>1</v>
+      </c>
+      <c r="F697">
+        <v>4</v>
+      </c>
+      <c r="G697" t="s">
+        <v>26</v>
+      </c>
+      <c r="H697" t="s">
+        <v>53</v>
+      </c>
+      <c r="J697" t="s">
+        <v>17</v>
+      </c>
+      <c r="K697" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="698" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A698" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B698" t="s">
+        <v>89</v>
+      </c>
+      <c r="C698" t="s">
+        <v>75</v>
+      </c>
+      <c r="D698" t="s">
+        <v>8</v>
+      </c>
+      <c r="E698">
+        <v>1</v>
+      </c>
+      <c r="F698">
+        <v>4</v>
+      </c>
+      <c r="G698" t="s">
+        <v>26</v>
+      </c>
+      <c r="H698" t="s">
+        <v>44</v>
+      </c>
+      <c r="J698" t="s">
+        <v>17</v>
+      </c>
+      <c r="K698" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="699" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A699" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B699" t="s">
+        <v>89</v>
+      </c>
+      <c r="C699" t="s">
+        <v>75</v>
+      </c>
+      <c r="D699" t="s">
+        <v>8</v>
+      </c>
+      <c r="E699">
+        <v>1</v>
+      </c>
+      <c r="F699">
+        <v>4</v>
+      </c>
+      <c r="G699" t="s">
+        <v>26</v>
+      </c>
+      <c r="H699" t="s">
+        <v>19</v>
+      </c>
+      <c r="J699" t="s">
+        <v>17</v>
+      </c>
+      <c r="K699" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="700" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A700" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B700" t="s">
+        <v>89</v>
+      </c>
+      <c r="C700" t="s">
+        <v>75</v>
+      </c>
+      <c r="D700" t="s">
+        <v>8</v>
+      </c>
+      <c r="E700">
+        <v>1</v>
+      </c>
+      <c r="F700">
+        <v>4</v>
+      </c>
+      <c r="G700" t="s">
+        <v>22</v>
+      </c>
+      <c r="H700" t="s">
+        <v>53</v>
+      </c>
+      <c r="J700" t="s">
+        <v>17</v>
+      </c>
+      <c r="K700" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="701" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A701" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B701" t="s">
+        <v>89</v>
+      </c>
+      <c r="C701" t="s">
+        <v>75</v>
+      </c>
+      <c r="D701" t="s">
+        <v>8</v>
+      </c>
+      <c r="E701">
+        <v>1</v>
+      </c>
+      <c r="F701">
+        <v>4</v>
+      </c>
+      <c r="G701" t="s">
+        <v>26</v>
+      </c>
+      <c r="H701" t="s">
+        <v>54</v>
+      </c>
+      <c r="J701" t="s">
+        <v>17</v>
+      </c>
+      <c r="K701" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="702" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A702" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B702" t="s">
+        <v>89</v>
+      </c>
+      <c r="C702" t="s">
+        <v>75</v>
+      </c>
+      <c r="D702" t="s">
+        <v>8</v>
+      </c>
+      <c r="E702">
+        <v>1</v>
+      </c>
+      <c r="F702">
+        <v>4</v>
+      </c>
+      <c r="G702" t="s">
+        <v>26</v>
+      </c>
+      <c r="H702" t="s">
+        <v>19</v>
+      </c>
+      <c r="J702" t="s">
+        <v>18</v>
+      </c>
+      <c r="K702" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="703" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A703" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B703" t="s">
+        <v>89</v>
+      </c>
+      <c r="C703" t="s">
+        <v>75</v>
+      </c>
+      <c r="D703" t="s">
+        <v>8</v>
+      </c>
+      <c r="E703">
+        <v>1</v>
+      </c>
+      <c r="F703">
+        <v>8</v>
+      </c>
+      <c r="G703" t="s">
+        <v>24</v>
+      </c>
+      <c r="H703" t="s">
+        <v>21</v>
+      </c>
+      <c r="J703" t="s">
+        <v>13</v>
+      </c>
+      <c r="K703" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="704" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A704" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B704" t="s">
+        <v>89</v>
+      </c>
+      <c r="C704" t="s">
+        <v>75</v>
+      </c>
+      <c r="D704" t="s">
+        <v>8</v>
+      </c>
+      <c r="E704">
+        <v>1</v>
+      </c>
+      <c r="F704">
+        <v>2</v>
+      </c>
+      <c r="G704" t="s">
+        <v>26</v>
+      </c>
+      <c r="H704" t="s">
+        <v>78</v>
+      </c>
+      <c r="J704" t="s">
+        <v>17</v>
+      </c>
+      <c r="K704" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="705" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A705" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B705" t="s">
+        <v>89</v>
+      </c>
+      <c r="C705" t="s">
+        <v>75</v>
+      </c>
+      <c r="D705" t="s">
+        <v>8</v>
+      </c>
+      <c r="E705">
+        <v>1</v>
+      </c>
+      <c r="F705">
+        <v>2</v>
+      </c>
+      <c r="G705" t="s">
+        <v>26</v>
+      </c>
+      <c r="H705" t="s">
+        <v>53</v>
+      </c>
+      <c r="J705" t="s">
+        <v>17</v>
+      </c>
+      <c r="K705" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="706" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A706" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B706" t="s">
+        <v>89</v>
+      </c>
+      <c r="C706" t="s">
+        <v>75</v>
+      </c>
+      <c r="D706" t="s">
+        <v>8</v>
+      </c>
+      <c r="E706">
+        <v>1</v>
+      </c>
+      <c r="F706">
+        <v>2</v>
+      </c>
+      <c r="G706" t="s">
+        <v>26</v>
+      </c>
+      <c r="H706" t="s">
+        <v>19</v>
+      </c>
+      <c r="J706" t="s">
+        <v>18</v>
+      </c>
+      <c r="K706" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="707" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A707" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B707" t="s">
+        <v>89</v>
+      </c>
+      <c r="C707" t="s">
+        <v>75</v>
+      </c>
+      <c r="D707" t="s">
+        <v>8</v>
+      </c>
+      <c r="E707">
+        <v>1</v>
+      </c>
+      <c r="F707">
+        <v>2</v>
+      </c>
+      <c r="G707" t="s">
+        <v>26</v>
+      </c>
+      <c r="H707" t="s">
+        <v>19</v>
+      </c>
+      <c r="J707" t="s">
+        <v>18</v>
+      </c>
+      <c r="K707" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="708" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A708" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B708" t="s">
+        <v>89</v>
+      </c>
+      <c r="C708" t="s">
+        <v>75</v>
+      </c>
+      <c r="D708" t="s">
+        <v>8</v>
+      </c>
+      <c r="E708">
+        <v>1</v>
+      </c>
+      <c r="F708">
+        <v>2</v>
+      </c>
+      <c r="G708" t="s">
+        <v>26</v>
+      </c>
+      <c r="H708" t="s">
+        <v>45</v>
+      </c>
+      <c r="J708" t="s">
+        <v>13</v>
+      </c>
+      <c r="K708" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="709" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A709" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B709" t="s">
+        <v>89</v>
+      </c>
+      <c r="C709" t="s">
+        <v>75</v>
+      </c>
+      <c r="D709" t="s">
+        <v>8</v>
+      </c>
+      <c r="E709">
+        <v>1</v>
+      </c>
+      <c r="F709">
+        <v>2</v>
+      </c>
+      <c r="G709" t="s">
+        <v>26</v>
+      </c>
+      <c r="H709" t="s">
+        <v>19</v>
+      </c>
+      <c r="J709" t="s">
+        <v>18</v>
+      </c>
+      <c r="K709" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="710" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A710" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B710" t="s">
+        <v>89</v>
+      </c>
+      <c r="C710" t="s">
+        <v>75</v>
+      </c>
+      <c r="D710" t="s">
+        <v>8</v>
+      </c>
+      <c r="E710">
+        <v>1</v>
+      </c>
+      <c r="F710">
+        <v>2</v>
+      </c>
+      <c r="G710" t="s">
+        <v>26</v>
+      </c>
+      <c r="H710" t="s">
+        <v>19</v>
+      </c>
+      <c r="J710" t="s">
+        <v>18</v>
+      </c>
+      <c r="K710" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="711" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A711" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B711" t="s">
+        <v>89</v>
+      </c>
+      <c r="C711" t="s">
+        <v>75</v>
+      </c>
+      <c r="D711" t="s">
+        <v>8</v>
+      </c>
+      <c r="E711">
+        <v>1</v>
+      </c>
+      <c r="F711">
+        <v>2</v>
+      </c>
+      <c r="G711" t="s">
+        <v>26</v>
+      </c>
+      <c r="H711" t="s">
+        <v>21</v>
+      </c>
+      <c r="J711" t="s">
+        <v>18</v>
+      </c>
+      <c r="K711" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="712" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A712" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B712" t="s">
+        <v>89</v>
+      </c>
+      <c r="C712" t="s">
+        <v>75</v>
+      </c>
+      <c r="D712" t="s">
+        <v>8</v>
+      </c>
+      <c r="E712">
+        <v>1</v>
+      </c>
+      <c r="F712">
+        <v>2</v>
+      </c>
+      <c r="G712" t="s">
+        <v>26</v>
+      </c>
+      <c r="H712" t="s">
+        <v>19</v>
+      </c>
+      <c r="J712" t="s">
+        <v>18</v>
+      </c>
+      <c r="K712" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="713" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A713" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B713" t="s">
+        <v>89</v>
+      </c>
+      <c r="C713" t="s">
+        <v>75</v>
+      </c>
+      <c r="D713" t="s">
+        <v>8</v>
+      </c>
+      <c r="E713">
+        <v>1</v>
+      </c>
+      <c r="F713">
+        <v>2</v>
+      </c>
+      <c r="G713" t="s">
+        <v>26</v>
+      </c>
+      <c r="H713" t="s">
+        <v>19</v>
+      </c>
+      <c r="J713" t="s">
+        <v>18</v>
+      </c>
+      <c r="K713" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="714" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A714" s="1">
+        <v>43333</v>
+      </c>
+      <c r="B714" t="s">
+        <v>89</v>
+      </c>
+      <c r="C714" t="s">
+        <v>75</v>
+      </c>
+      <c r="D714" t="s">
+        <v>8</v>
+      </c>
+      <c r="E714">
+        <v>1</v>
+      </c>
+      <c r="F714">
+        <v>2</v>
+      </c>
+      <c r="G714" t="s">
+        <v>26</v>
+      </c>
+      <c r="H714" t="s">
+        <v>25</v>
+      </c>
+      <c r="I714" t="s">
+        <v>29</v>
+      </c>
+      <c r="J714" t="s">
+        <v>13</v>
+      </c>
+      <c r="K714" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="715" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A715" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B715" t="s">
+        <v>89</v>
+      </c>
+      <c r="C715" t="s">
+        <v>76</v>
+      </c>
+      <c r="D715" t="s">
+        <v>60</v>
+      </c>
+      <c r="E715">
+        <v>1</v>
+      </c>
+      <c r="F715">
+        <v>7</v>
+      </c>
+      <c r="G715" t="s">
+        <v>26</v>
+      </c>
+      <c r="H715" t="s">
+        <v>20</v>
+      </c>
+      <c r="J715" t="s">
+        <v>17</v>
+      </c>
+      <c r="K715" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="716" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A716" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B716" t="s">
+        <v>89</v>
+      </c>
+      <c r="C716" t="s">
+        <v>76</v>
+      </c>
+      <c r="D716" t="s">
+        <v>60</v>
+      </c>
+      <c r="E716">
+        <v>1</v>
+      </c>
+      <c r="F716">
+        <v>7</v>
+      </c>
+      <c r="G716" t="s">
+        <v>26</v>
+      </c>
+      <c r="H716" t="s">
+        <v>47</v>
+      </c>
+      <c r="J716" t="s">
+        <v>17</v>
+      </c>
+      <c r="K716" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="717" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A717" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B717" t="s">
+        <v>89</v>
+      </c>
+      <c r="C717" t="s">
+        <v>76</v>
+      </c>
+      <c r="D717" t="s">
+        <v>60</v>
+      </c>
+      <c r="E717">
+        <v>1</v>
+      </c>
+      <c r="F717">
+        <v>7</v>
+      </c>
+      <c r="G717" t="s">
+        <v>26</v>
+      </c>
+      <c r="H717" t="s">
+        <v>19</v>
+      </c>
+      <c r="I717" t="s">
+        <v>15</v>
+      </c>
+      <c r="J717" t="s">
+        <v>13</v>
+      </c>
+      <c r="K717" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="718" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A718" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B718" t="s">
+        <v>89</v>
+      </c>
+      <c r="C718" t="s">
+        <v>76</v>
+      </c>
+      <c r="D718" t="s">
+        <v>60</v>
+      </c>
+      <c r="E718">
+        <v>1</v>
+      </c>
+      <c r="F718">
+        <v>7</v>
+      </c>
+      <c r="G718" t="s">
+        <v>26</v>
+      </c>
+      <c r="H718" t="s">
+        <v>45</v>
+      </c>
+      <c r="J718" t="s">
+        <v>13</v>
+      </c>
+      <c r="K718" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="719" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A719" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B719" t="s">
+        <v>89</v>
+      </c>
+      <c r="C719" t="s">
+        <v>76</v>
+      </c>
+      <c r="D719" t="s">
+        <v>60</v>
+      </c>
+      <c r="E719">
+        <v>1</v>
+      </c>
+      <c r="F719">
+        <v>7</v>
+      </c>
+      <c r="G719" t="s">
+        <v>26</v>
+      </c>
+      <c r="H719" t="s">
+        <v>19</v>
+      </c>
+      <c r="J719" t="s">
+        <v>17</v>
+      </c>
+      <c r="K719" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="720" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A720" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B720" t="s">
+        <v>89</v>
+      </c>
+      <c r="C720" t="s">
+        <v>76</v>
+      </c>
+      <c r="D720" t="s">
+        <v>60</v>
+      </c>
+      <c r="E720">
+        <v>1</v>
+      </c>
+      <c r="F720">
+        <v>7</v>
+      </c>
+      <c r="G720" t="s">
+        <v>26</v>
+      </c>
+      <c r="H720" t="s">
+        <v>25</v>
+      </c>
+      <c r="I720" t="s">
+        <v>59</v>
+      </c>
+      <c r="J720" t="s">
+        <v>13</v>
+      </c>
+      <c r="K720" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="721" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A721" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B721" t="s">
+        <v>89</v>
+      </c>
+      <c r="C721" t="s">
+        <v>76</v>
+      </c>
+      <c r="D721" t="s">
+        <v>60</v>
+      </c>
+      <c r="E721">
+        <v>1</v>
+      </c>
+      <c r="F721">
+        <v>7</v>
+      </c>
+      <c r="G721" t="s">
+        <v>26</v>
+      </c>
+      <c r="H721" t="s">
+        <v>21</v>
+      </c>
+      <c r="I721" t="s">
+        <v>41</v>
+      </c>
+      <c r="J721" t="s">
+        <v>13</v>
+      </c>
+      <c r="K721" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="722" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A722" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B722" t="s">
+        <v>89</v>
+      </c>
+      <c r="C722" t="s">
+        <v>76</v>
+      </c>
+      <c r="D722" t="s">
+        <v>60</v>
+      </c>
+      <c r="E722">
+        <v>1</v>
+      </c>
+      <c r="F722">
+        <v>7</v>
+      </c>
+      <c r="G722" t="s">
+        <v>26</v>
+      </c>
+      <c r="H722" t="s">
+        <v>53</v>
+      </c>
+      <c r="J722" t="s">
+        <v>17</v>
+      </c>
+      <c r="K722" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="723" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A723" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B723" t="s">
+        <v>89</v>
+      </c>
+      <c r="C723" t="s">
+        <v>76</v>
+      </c>
+      <c r="D723" t="s">
+        <v>60</v>
+      </c>
+      <c r="E723">
+        <v>1</v>
+      </c>
+      <c r="F723">
+        <v>2</v>
+      </c>
+      <c r="G723" t="s">
+        <v>26</v>
+      </c>
+      <c r="H723" t="s">
+        <v>19</v>
+      </c>
+      <c r="J723" t="s">
+        <v>18</v>
+      </c>
+      <c r="K723" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="724" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A724" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B724" t="s">
+        <v>89</v>
+      </c>
+      <c r="C724" t="s">
+        <v>76</v>
+      </c>
+      <c r="D724" t="s">
+        <v>60</v>
+      </c>
+      <c r="E724">
+        <v>1</v>
+      </c>
+      <c r="F724">
+        <v>2</v>
+      </c>
+      <c r="G724" t="s">
+        <v>24</v>
+      </c>
+      <c r="H724" t="s">
+        <v>44</v>
+      </c>
+      <c r="J724" t="s">
+        <v>17</v>
+      </c>
+      <c r="K724" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="725" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A725" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B725" t="s">
+        <v>89</v>
+      </c>
+      <c r="C725" t="s">
+        <v>76</v>
+      </c>
+      <c r="D725" t="s">
+        <v>60</v>
+      </c>
+      <c r="E725">
+        <v>1</v>
+      </c>
+      <c r="F725">
+        <v>2</v>
+      </c>
+      <c r="G725" t="s">
+        <v>26</v>
+      </c>
+      <c r="H725" t="s">
+        <v>31</v>
+      </c>
+      <c r="I725" t="s">
+        <v>30</v>
+      </c>
+      <c r="J725" t="s">
+        <v>13</v>
+      </c>
+      <c r="K725" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="726" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A726" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B726" t="s">
+        <v>89</v>
+      </c>
+      <c r="C726" t="s">
+        <v>76</v>
+      </c>
+      <c r="D726" t="s">
+        <v>60</v>
+      </c>
+      <c r="E726">
+        <v>1</v>
+      </c>
+      <c r="F726">
+        <v>2</v>
+      </c>
+      <c r="G726" t="s">
+        <v>26</v>
+      </c>
+      <c r="H726" t="s">
+        <v>21</v>
+      </c>
+      <c r="I726" t="s">
+        <v>70</v>
+      </c>
+      <c r="J726" t="s">
+        <v>13</v>
+      </c>
+      <c r="K726" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="727" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A727" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B727" t="s">
+        <v>89</v>
+      </c>
+      <c r="C727" t="s">
+        <v>76</v>
+      </c>
+      <c r="D727" t="s">
+        <v>60</v>
+      </c>
+      <c r="E727">
+        <v>1</v>
+      </c>
+      <c r="F727">
+        <v>2</v>
+      </c>
+      <c r="G727" t="s">
+        <v>26</v>
+      </c>
+      <c r="H727" t="s">
+        <v>54</v>
+      </c>
+      <c r="J727" t="s">
+        <v>17</v>
+      </c>
+      <c r="K727" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="728" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A728" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B728" t="s">
+        <v>89</v>
+      </c>
+      <c r="C728" t="s">
+        <v>76</v>
+      </c>
+      <c r="D728" t="s">
+        <v>60</v>
+      </c>
+      <c r="E728">
+        <v>1</v>
+      </c>
+      <c r="F728">
+        <v>2</v>
+      </c>
+      <c r="G728" t="s">
+        <v>24</v>
+      </c>
+      <c r="H728" t="s">
+        <v>54</v>
+      </c>
+      <c r="J728" t="s">
+        <v>17</v>
+      </c>
+      <c r="K728" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="729" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A729" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B729" t="s">
+        <v>89</v>
+      </c>
+      <c r="C729" t="s">
+        <v>76</v>
+      </c>
+      <c r="D729" t="s">
+        <v>60</v>
+      </c>
+      <c r="E729">
+        <v>1</v>
+      </c>
+      <c r="F729">
+        <v>2</v>
+      </c>
+      <c r="G729" t="s">
+        <v>26</v>
+      </c>
+      <c r="H729" t="s">
+        <v>34</v>
+      </c>
+      <c r="I729" t="s">
+        <v>64</v>
+      </c>
+      <c r="J729" t="s">
+        <v>18</v>
+      </c>
+      <c r="K729" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="730" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A730" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B730" t="s">
+        <v>89</v>
+      </c>
+      <c r="C730" t="s">
+        <v>76</v>
+      </c>
+      <c r="D730" t="s">
+        <v>60</v>
+      </c>
+      <c r="E730">
+        <v>1</v>
+      </c>
+      <c r="F730">
+        <v>2</v>
+      </c>
+      <c r="G730" t="s">
+        <v>26</v>
+      </c>
+      <c r="H730" t="s">
+        <v>31</v>
+      </c>
+      <c r="I730" t="s">
+        <v>30</v>
+      </c>
+      <c r="J730" t="s">
+        <v>13</v>
+      </c>
+      <c r="K730" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="731" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A731" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B731" t="s">
+        <v>89</v>
+      </c>
+      <c r="C731" t="s">
+        <v>76</v>
+      </c>
+      <c r="D731" t="s">
+        <v>60</v>
+      </c>
+      <c r="E731">
+        <v>1</v>
+      </c>
+      <c r="F731">
+        <v>2</v>
+      </c>
+      <c r="G731" t="s">
+        <v>26</v>
+      </c>
+      <c r="H731" t="s">
+        <v>44</v>
+      </c>
+      <c r="J731" t="s">
+        <v>17</v>
+      </c>
+      <c r="K731" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="732" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A732" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B732" t="s">
+        <v>89</v>
+      </c>
+      <c r="C732" t="s">
+        <v>76</v>
+      </c>
+      <c r="D732" t="s">
+        <v>60</v>
+      </c>
+      <c r="E732">
+        <v>1</v>
+      </c>
+      <c r="F732">
+        <v>1</v>
+      </c>
+      <c r="G732" t="s">
+        <v>26</v>
+      </c>
+      <c r="H732" t="s">
+        <v>21</v>
+      </c>
+      <c r="I732" t="s">
+        <v>41</v>
+      </c>
+      <c r="J732" t="s">
+        <v>18</v>
+      </c>
+      <c r="K732" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="733" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A733" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B733" t="s">
+        <v>89</v>
+      </c>
+      <c r="C733" t="s">
+        <v>76</v>
+      </c>
+      <c r="D733" t="s">
+        <v>60</v>
+      </c>
+      <c r="E733">
+        <v>1</v>
+      </c>
+      <c r="F733">
+        <v>1</v>
+      </c>
+      <c r="G733" t="s">
+        <v>26</v>
+      </c>
+      <c r="H733" t="s">
+        <v>21</v>
+      </c>
+      <c r="I733" t="s">
+        <v>56</v>
+      </c>
+      <c r="J733" t="s">
+        <v>13</v>
+      </c>
+      <c r="K733" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="734" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A734" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B734" t="s">
+        <v>89</v>
+      </c>
+      <c r="C734" t="s">
+        <v>76</v>
+      </c>
+      <c r="D734" t="s">
+        <v>60</v>
+      </c>
+      <c r="E734">
+        <v>1</v>
+      </c>
+      <c r="F734">
+        <v>1</v>
+      </c>
+      <c r="G734" t="s">
+        <v>26</v>
+      </c>
+      <c r="H734" t="s">
+        <v>19</v>
+      </c>
+      <c r="I734" t="s">
+        <v>57</v>
+      </c>
+      <c r="J734" t="s">
+        <v>13</v>
+      </c>
+      <c r="K734" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="735" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A735" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B735" t="s">
+        <v>89</v>
+      </c>
+      <c r="C735" t="s">
+        <v>76</v>
+      </c>
+      <c r="D735" t="s">
+        <v>60</v>
+      </c>
+      <c r="E735">
+        <v>1</v>
+      </c>
+      <c r="F735">
+        <v>1</v>
+      </c>
+      <c r="G735" t="s">
+        <v>26</v>
+      </c>
+      <c r="H735" t="s">
+        <v>25</v>
+      </c>
+      <c r="I735" t="s">
+        <v>29</v>
+      </c>
+      <c r="J735" t="s">
+        <v>13</v>
+      </c>
+      <c r="K735" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="736" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A736" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B736" t="s">
+        <v>89</v>
+      </c>
+      <c r="C736" t="s">
+        <v>76</v>
+      </c>
+      <c r="D736" t="s">
+        <v>60</v>
+      </c>
+      <c r="E736">
+        <v>1</v>
+      </c>
+      <c r="F736">
+        <v>1</v>
+      </c>
+      <c r="G736" t="s">
+        <v>26</v>
+      </c>
+      <c r="H736" t="s">
+        <v>19</v>
+      </c>
+      <c r="I736" t="s">
+        <v>15</v>
+      </c>
+      <c r="J736" t="s">
+        <v>13</v>
+      </c>
+      <c r="K736" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="737" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A737" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B737" t="s">
+        <v>89</v>
+      </c>
+      <c r="C737" t="s">
+        <v>76</v>
+      </c>
+      <c r="D737" t="s">
+        <v>60</v>
+      </c>
+      <c r="E737">
+        <v>1</v>
+      </c>
+      <c r="F737">
+        <v>1</v>
+      </c>
+      <c r="G737" t="s">
+        <v>26</v>
+      </c>
+      <c r="H737" t="s">
+        <v>19</v>
+      </c>
+      <c r="I737" t="s">
+        <v>92</v>
+      </c>
+      <c r="J737" t="s">
+        <v>13</v>
+      </c>
+      <c r="K737" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="738" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A738" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B738" t="s">
+        <v>89</v>
+      </c>
+      <c r="C738" t="s">
+        <v>76</v>
+      </c>
+      <c r="D738" t="s">
+        <v>60</v>
+      </c>
+      <c r="E738">
+        <v>1</v>
+      </c>
+      <c r="F738">
+        <v>1</v>
+      </c>
+      <c r="G738" t="s">
+        <v>26</v>
+      </c>
+      <c r="H738" t="s">
+        <v>93</v>
+      </c>
+      <c r="I738" t="s">
+        <v>92</v>
+      </c>
+      <c r="J738" t="s">
+        <v>13</v>
+      </c>
+      <c r="K738" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="739" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A739" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B739" t="s">
+        <v>89</v>
+      </c>
+      <c r="C739" t="s">
+        <v>76</v>
+      </c>
+      <c r="D739" t="s">
+        <v>60</v>
+      </c>
+      <c r="E739">
+        <v>1</v>
+      </c>
+      <c r="F739">
+        <v>1</v>
+      </c>
+      <c r="G739" t="s">
+        <v>26</v>
+      </c>
+      <c r="H739" t="s">
+        <v>44</v>
+      </c>
+      <c r="J739" t="s">
+        <v>17</v>
+      </c>
+      <c r="K739" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="740" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A740" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B740" t="s">
+        <v>89</v>
+      </c>
+      <c r="C740" t="s">
+        <v>76</v>
+      </c>
+      <c r="D740" t="s">
+        <v>60</v>
+      </c>
+      <c r="E740">
+        <v>1</v>
+      </c>
+      <c r="F740">
+        <v>1</v>
+      </c>
+      <c r="G740" t="s">
+        <v>26</v>
+      </c>
+      <c r="H740" t="s">
+        <v>21</v>
+      </c>
+      <c r="J740" t="s">
+        <v>18</v>
+      </c>
+      <c r="K740" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="741" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A741" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B741" t="s">
+        <v>89</v>
+      </c>
+      <c r="C741" t="s">
+        <v>76</v>
+      </c>
+      <c r="D741" t="s">
+        <v>60</v>
+      </c>
+      <c r="E741">
+        <v>1</v>
+      </c>
+      <c r="F741">
+        <v>1</v>
+      </c>
+      <c r="G741" t="s">
+        <v>26</v>
+      </c>
+      <c r="H741" t="s">
+        <v>21</v>
+      </c>
+      <c r="J741" t="s">
+        <v>18</v>
+      </c>
+      <c r="K741" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="742" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A742" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B742" t="s">
+        <v>89</v>
+      </c>
+      <c r="C742" t="s">
+        <v>76</v>
+      </c>
+      <c r="D742" t="s">
+        <v>60</v>
+      </c>
+      <c r="E742">
+        <v>1</v>
+      </c>
+      <c r="F742">
+        <v>1</v>
+      </c>
+      <c r="G742" t="s">
+        <v>26</v>
+      </c>
+      <c r="H742" t="s">
+        <v>54</v>
+      </c>
+      <c r="J742" t="s">
+        <v>17</v>
+      </c>
+      <c r="K742" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="743" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A743" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B743" t="s">
+        <v>89</v>
+      </c>
+      <c r="C743" t="s">
+        <v>76</v>
+      </c>
+      <c r="D743" t="s">
+        <v>60</v>
+      </c>
+      <c r="E743">
+        <v>1</v>
+      </c>
+      <c r="F743">
+        <v>1</v>
+      </c>
+      <c r="G743" t="s">
+        <v>24</v>
+      </c>
+      <c r="H743" t="s">
+        <v>54</v>
+      </c>
+      <c r="J743" t="s">
+        <v>17</v>
+      </c>
+      <c r="K743" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="744" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A744" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B744" t="s">
+        <v>89</v>
+      </c>
+      <c r="C744" t="s">
+        <v>76</v>
+      </c>
+      <c r="D744" t="s">
+        <v>60</v>
+      </c>
+      <c r="E744">
+        <v>1</v>
+      </c>
+      <c r="F744">
+        <v>1</v>
+      </c>
+      <c r="G744" t="s">
+        <v>26</v>
+      </c>
+      <c r="H744" t="s">
+        <v>44</v>
+      </c>
+      <c r="J744" t="s">
+        <v>17</v>
+      </c>
+      <c r="K744" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="745" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A745" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B745" t="s">
+        <v>89</v>
+      </c>
+      <c r="C745" t="s">
+        <v>76</v>
+      </c>
+      <c r="D745" t="s">
+        <v>60</v>
+      </c>
+      <c r="E745">
+        <v>1</v>
+      </c>
+      <c r="F745">
+        <v>1</v>
+      </c>
+      <c r="G745" t="s">
+        <v>26</v>
+      </c>
+      <c r="H745" t="s">
+        <v>44</v>
+      </c>
+      <c r="J745" t="s">
+        <v>17</v>
+      </c>
+      <c r="K745" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="746" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A746" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B746" t="s">
+        <v>89</v>
+      </c>
+      <c r="C746" t="s">
+        <v>76</v>
+      </c>
+      <c r="D746" t="s">
+        <v>60</v>
+      </c>
+      <c r="E746">
+        <v>1</v>
+      </c>
+      <c r="F746">
+        <v>1</v>
+      </c>
+      <c r="G746" t="s">
+        <v>26</v>
+      </c>
+      <c r="H746" t="s">
+        <v>54</v>
+      </c>
+      <c r="J746" t="s">
+        <v>17</v>
+      </c>
+      <c r="K746" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="747" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A747" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B747" t="s">
+        <v>89</v>
+      </c>
+      <c r="C747" t="s">
+        <v>76</v>
+      </c>
+      <c r="D747" t="s">
+        <v>60</v>
+      </c>
+      <c r="E747">
+        <v>1</v>
+      </c>
+      <c r="F747">
+        <v>1</v>
+      </c>
+      <c r="G747" t="s">
+        <v>26</v>
+      </c>
+      <c r="H747" t="s">
+        <v>21</v>
+      </c>
+      <c r="I747" t="s">
+        <v>56</v>
+      </c>
+      <c r="J747" t="s">
+        <v>13</v>
+      </c>
+      <c r="K747" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="748" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A748" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B748" t="s">
+        <v>89</v>
+      </c>
+      <c r="C748" t="s">
+        <v>76</v>
+      </c>
+      <c r="D748" t="s">
+        <v>60</v>
+      </c>
+      <c r="E748">
+        <v>1</v>
+      </c>
+      <c r="F748">
+        <v>1</v>
+      </c>
+      <c r="G748" t="s">
+        <v>26</v>
+      </c>
+      <c r="H748" t="s">
+        <v>25</v>
+      </c>
+      <c r="I748" t="s">
+        <v>29</v>
+      </c>
+      <c r="J748" t="s">
+        <v>13</v>
+      </c>
+      <c r="K748" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="749" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A749" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B749" t="s">
+        <v>89</v>
+      </c>
+      <c r="C749" t="s">
+        <v>76</v>
+      </c>
+      <c r="D749" t="s">
+        <v>60</v>
+      </c>
+      <c r="E749">
+        <v>1</v>
+      </c>
+      <c r="F749">
+        <v>1</v>
+      </c>
+      <c r="G749" t="s">
+        <v>24</v>
+      </c>
+      <c r="H749" t="s">
+        <v>21</v>
+      </c>
+      <c r="J749" t="s">
+        <v>18</v>
+      </c>
+      <c r="K749" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="750" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A750" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B750" t="s">
+        <v>89</v>
+      </c>
+      <c r="C750" t="s">
+        <v>76</v>
+      </c>
+      <c r="D750" t="s">
+        <v>60</v>
+      </c>
+      <c r="E750">
+        <v>1</v>
+      </c>
+      <c r="F750">
+        <v>4</v>
+      </c>
+      <c r="G750" t="s">
+        <v>26</v>
+      </c>
+      <c r="H750" t="s">
+        <v>31</v>
+      </c>
+      <c r="I750" t="s">
+        <v>37</v>
+      </c>
+      <c r="J750" t="s">
+        <v>13</v>
+      </c>
+      <c r="K750" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="751" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A751" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B751" t="s">
+        <v>89</v>
+      </c>
+      <c r="C751" t="s">
+        <v>76</v>
+      </c>
+      <c r="D751" t="s">
+        <v>60</v>
+      </c>
+      <c r="E751">
+        <v>1</v>
+      </c>
+      <c r="F751">
+        <v>4</v>
+      </c>
+      <c r="G751" t="s">
+        <v>26</v>
+      </c>
+      <c r="H751" t="s">
+        <v>19</v>
+      </c>
+      <c r="J751" t="s">
+        <v>18</v>
+      </c>
+      <c r="K751" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="752" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A752" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B752" t="s">
+        <v>89</v>
+      </c>
+      <c r="C752" t="s">
+        <v>76</v>
+      </c>
+      <c r="D752" t="s">
+        <v>60</v>
+      </c>
+      <c r="E752">
+        <v>1</v>
+      </c>
+      <c r="F752">
+        <v>4</v>
+      </c>
+      <c r="G752" t="s">
+        <v>26</v>
+      </c>
+      <c r="H752" t="s">
+        <v>19</v>
+      </c>
+      <c r="I752" t="s">
+        <v>15</v>
+      </c>
+      <c r="J752" t="s">
+        <v>13</v>
+      </c>
+      <c r="K752" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="753" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A753" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B753" t="s">
+        <v>89</v>
+      </c>
+      <c r="C753" t="s">
+        <v>76</v>
+      </c>
+      <c r="D753" t="s">
+        <v>60</v>
+      </c>
+      <c r="E753">
+        <v>1</v>
+      </c>
+      <c r="F753">
+        <v>4</v>
+      </c>
+      <c r="G753" t="s">
+        <v>26</v>
+      </c>
+      <c r="H753" t="s">
+        <v>20</v>
+      </c>
+      <c r="I753" t="s">
+        <v>94</v>
+      </c>
+      <c r="J753" t="s">
+        <v>18</v>
+      </c>
+      <c r="K753" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="754" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A754" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B754" t="s">
+        <v>89</v>
+      </c>
+      <c r="C754" t="s">
+        <v>76</v>
+      </c>
+      <c r="D754" t="s">
+        <v>60</v>
+      </c>
+      <c r="E754">
+        <v>1</v>
+      </c>
+      <c r="F754">
+        <v>4</v>
+      </c>
+      <c r="G754" t="s">
+        <v>26</v>
+      </c>
+      <c r="H754" t="s">
+        <v>21</v>
+      </c>
+      <c r="I754" t="s">
+        <v>41</v>
+      </c>
+      <c r="J754" t="s">
+        <v>13</v>
+      </c>
+      <c r="K754" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="755" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A755" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B755" t="s">
+        <v>89</v>
+      </c>
+      <c r="C755" t="s">
+        <v>76</v>
+      </c>
+      <c r="D755" t="s">
+        <v>60</v>
+      </c>
+      <c r="E755">
+        <v>1</v>
+      </c>
+      <c r="F755">
+        <v>4</v>
+      </c>
+      <c r="G755" t="s">
+        <v>26</v>
+      </c>
+      <c r="H755" t="s">
+        <v>19</v>
+      </c>
+      <c r="J755" t="s">
+        <v>18</v>
+      </c>
+      <c r="K755" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="756" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A756" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B756" t="s">
+        <v>89</v>
+      </c>
+      <c r="C756" t="s">
+        <v>76</v>
+      </c>
+      <c r="D756" t="s">
+        <v>60</v>
+      </c>
+      <c r="E756">
+        <v>1</v>
+      </c>
+      <c r="F756">
+        <v>6</v>
+      </c>
+      <c r="G756" t="s">
+        <v>26</v>
+      </c>
+      <c r="H756" t="s">
+        <v>25</v>
+      </c>
+      <c r="I756" t="s">
+        <v>29</v>
+      </c>
+      <c r="J756" t="s">
+        <v>13</v>
+      </c>
+      <c r="K756" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="757" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A757" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B757" t="s">
+        <v>89</v>
+      </c>
+      <c r="C757" t="s">
+        <v>76</v>
+      </c>
+      <c r="D757" t="s">
+        <v>60</v>
+      </c>
+      <c r="E757">
+        <v>1</v>
+      </c>
+      <c r="F757">
+        <v>6</v>
+      </c>
+      <c r="G757" t="s">
+        <v>26</v>
+      </c>
+      <c r="H757" t="s">
+        <v>19</v>
+      </c>
+      <c r="J757" t="s">
+        <v>18</v>
+      </c>
+      <c r="K757" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="758" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A758" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B758" t="s">
+        <v>89</v>
+      </c>
+      <c r="C758" t="s">
+        <v>76</v>
+      </c>
+      <c r="D758" t="s">
+        <v>60</v>
+      </c>
+      <c r="E758">
+        <v>1</v>
+      </c>
+      <c r="F758">
+        <v>6</v>
+      </c>
+      <c r="G758" t="s">
+        <v>26</v>
+      </c>
+      <c r="H758" t="s">
+        <v>20</v>
+      </c>
+      <c r="J758" t="s">
+        <v>17</v>
+      </c>
+      <c r="K758" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="759" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A759" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B759" t="s">
+        <v>89</v>
+      </c>
+      <c r="C759" t="s">
+        <v>76</v>
+      </c>
+      <c r="D759" t="s">
+        <v>60</v>
+      </c>
+      <c r="E759">
+        <v>1</v>
+      </c>
+      <c r="F759">
+        <v>6</v>
+      </c>
+      <c r="G759" t="s">
+        <v>26</v>
+      </c>
+      <c r="H759" t="s">
+        <v>21</v>
+      </c>
+      <c r="I759" t="s">
+        <v>49</v>
+      </c>
+      <c r="J759" t="s">
+        <v>18</v>
+      </c>
+      <c r="K759" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="760" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A760" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B760" t="s">
+        <v>89</v>
+      </c>
+      <c r="C760" t="s">
+        <v>76</v>
+      </c>
+      <c r="D760" t="s">
+        <v>60</v>
+      </c>
+      <c r="E760">
+        <v>1</v>
+      </c>
+      <c r="F760">
+        <v>6</v>
+      </c>
+      <c r="G760" t="s">
+        <v>26</v>
+      </c>
+      <c r="H760" t="s">
+        <v>19</v>
+      </c>
+      <c r="J760" t="s">
+        <v>18</v>
+      </c>
+      <c r="K760" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="761" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A761" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B761" t="s">
+        <v>89</v>
+      </c>
+      <c r="C761" t="s">
+        <v>76</v>
+      </c>
+      <c r="D761" t="s">
+        <v>60</v>
+      </c>
+      <c r="E761">
+        <v>1</v>
+      </c>
+      <c r="F761">
+        <v>8</v>
+      </c>
+      <c r="G761" t="s">
+        <v>26</v>
+      </c>
+      <c r="H761" t="s">
+        <v>25</v>
+      </c>
+      <c r="I761" t="s">
+        <v>59</v>
+      </c>
+      <c r="J761" t="s">
+        <v>13</v>
+      </c>
+      <c r="K761" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="762" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A762" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B762" t="s">
+        <v>89</v>
+      </c>
+      <c r="C762" t="s">
+        <v>76</v>
+      </c>
+      <c r="D762" t="s">
+        <v>60</v>
+      </c>
+      <c r="E762">
+        <v>1</v>
+      </c>
+      <c r="F762">
+        <v>8</v>
+      </c>
+      <c r="G762" t="s">
+        <v>26</v>
+      </c>
+      <c r="H762" t="s">
+        <v>53</v>
+      </c>
+      <c r="J762" t="s">
+        <v>17</v>
+      </c>
+      <c r="K762" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="763" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A763" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B763" t="s">
+        <v>89</v>
+      </c>
+      <c r="C763" t="s">
+        <v>76</v>
+      </c>
+      <c r="D763" t="s">
+        <v>60</v>
+      </c>
+      <c r="E763">
+        <v>1</v>
+      </c>
+      <c r="F763">
+        <v>8</v>
+      </c>
+      <c r="G763" t="s">
+        <v>26</v>
+      </c>
+      <c r="H763" t="s">
+        <v>19</v>
+      </c>
+      <c r="I763" t="s">
+        <v>92</v>
+      </c>
+      <c r="J763" t="s">
+        <v>13</v>
+      </c>
+      <c r="K763" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="764" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A764" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B764" t="s">
+        <v>89</v>
+      </c>
+      <c r="C764" t="s">
+        <v>76</v>
+      </c>
+      <c r="D764" t="s">
+        <v>60</v>
+      </c>
+      <c r="E764">
+        <v>1</v>
+      </c>
+      <c r="F764">
+        <v>8</v>
+      </c>
+      <c r="G764" t="s">
+        <v>26</v>
+      </c>
+      <c r="H764" t="s">
+        <v>19</v>
+      </c>
+      <c r="I764" t="s">
+        <v>42</v>
+      </c>
+      <c r="J764" t="s">
+        <v>13</v>
+      </c>
+      <c r="K764" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="765" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A765" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B765" t="s">
+        <v>89</v>
+      </c>
+      <c r="C765" t="s">
+        <v>76</v>
+      </c>
+      <c r="D765" t="s">
+        <v>60</v>
+      </c>
+      <c r="E765">
+        <v>1</v>
+      </c>
+      <c r="F765">
+        <v>8</v>
+      </c>
+      <c r="G765" t="s">
+        <v>26</v>
+      </c>
+      <c r="H765" t="s">
+        <v>19</v>
+      </c>
+      <c r="J765" t="s">
+        <v>18</v>
+      </c>
+      <c r="K765" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="766" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A766" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B766" t="s">
+        <v>89</v>
+      </c>
+      <c r="C766" t="s">
+        <v>76</v>
+      </c>
+      <c r="D766" t="s">
+        <v>60</v>
+      </c>
+      <c r="E766">
+        <v>1</v>
+      </c>
+      <c r="F766">
+        <v>3</v>
+      </c>
+      <c r="G766" t="s">
+        <v>26</v>
+      </c>
+      <c r="H766" t="s">
+        <v>47</v>
+      </c>
+      <c r="J766" t="s">
+        <v>17</v>
+      </c>
+      <c r="K766" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="767" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A767" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B767" t="s">
+        <v>89</v>
+      </c>
+      <c r="C767" t="s">
+        <v>76</v>
+      </c>
+      <c r="D767" t="s">
+        <v>60</v>
+      </c>
+      <c r="E767">
+        <v>1</v>
+      </c>
+      <c r="F767">
+        <v>3</v>
+      </c>
+      <c r="G767" t="s">
+        <v>26</v>
+      </c>
+      <c r="H767" t="s">
+        <v>45</v>
+      </c>
+      <c r="J767" t="s">
+        <v>13</v>
+      </c>
+      <c r="K767" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="768" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A768" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B768" t="s">
+        <v>89</v>
+      </c>
+      <c r="C768" t="s">
+        <v>76</v>
+      </c>
+      <c r="D768" t="s">
+        <v>60</v>
+      </c>
+      <c r="E768">
+        <v>1</v>
+      </c>
+      <c r="F768">
+        <v>3</v>
+      </c>
+      <c r="G768" t="s">
+        <v>24</v>
+      </c>
+      <c r="H768" t="s">
+        <v>21</v>
+      </c>
+      <c r="J768" t="s">
+        <v>13</v>
+      </c>
+      <c r="K768" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="769" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A769" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B769" t="s">
+        <v>89</v>
+      </c>
+      <c r="C769" t="s">
+        <v>76</v>
+      </c>
+      <c r="D769" t="s">
+        <v>60</v>
+      </c>
+      <c r="E769">
+        <v>1</v>
+      </c>
+      <c r="F769">
+        <v>3</v>
+      </c>
+      <c r="G769" t="s">
+        <v>24</v>
+      </c>
+      <c r="H769" t="s">
+        <v>21</v>
+      </c>
+      <c r="J769" t="s">
+        <v>13</v>
+      </c>
+      <c r="K769" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="770" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A770" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B770" t="s">
+        <v>89</v>
+      </c>
+      <c r="C770" t="s">
+        <v>76</v>
+      </c>
+      <c r="D770" t="s">
+        <v>60</v>
+      </c>
+      <c r="E770">
+        <v>1</v>
+      </c>
+      <c r="F770">
+        <v>5</v>
+      </c>
+      <c r="G770" t="s">
+        <v>24</v>
+      </c>
+      <c r="H770" t="s">
+        <v>34</v>
+      </c>
+      <c r="I770" t="s">
+        <v>35</v>
+      </c>
+      <c r="J770" t="s">
+        <v>13</v>
+      </c>
+      <c r="K770" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="771" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A771" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B771" t="s">
+        <v>89</v>
+      </c>
+      <c r="C771" t="s">
+        <v>76</v>
+      </c>
+      <c r="D771" t="s">
+        <v>60</v>
+      </c>
+      <c r="E771">
+        <v>1</v>
+      </c>
+      <c r="F771">
+        <v>5</v>
+      </c>
+      <c r="G771" t="s">
+        <v>22</v>
+      </c>
+      <c r="H771" t="s">
+        <v>53</v>
+      </c>
+      <c r="J771" t="s">
+        <v>17</v>
+      </c>
+      <c r="K771" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="772" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A772" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B772" t="s">
+        <v>89</v>
+      </c>
+      <c r="C772" t="s">
+        <v>76</v>
+      </c>
+      <c r="D772" t="s">
+        <v>60</v>
+      </c>
+      <c r="E772">
+        <v>1</v>
+      </c>
+      <c r="F772">
+        <v>5</v>
+      </c>
+      <c r="G772" t="s">
+        <v>22</v>
+      </c>
+      <c r="H772" t="s">
+        <v>44</v>
+      </c>
+      <c r="J772" t="s">
+        <v>17</v>
+      </c>
+      <c r="K772" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="773" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A773" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B773" t="s">
+        <v>89</v>
+      </c>
+      <c r="C773" t="s">
+        <v>76</v>
+      </c>
+      <c r="D773" t="s">
+        <v>60</v>
+      </c>
+      <c r="E773">
+        <v>1</v>
+      </c>
+      <c r="F773">
+        <v>5</v>
+      </c>
+      <c r="G773" t="s">
+        <v>26</v>
+      </c>
+      <c r="H773" t="s">
+        <v>19</v>
+      </c>
+      <c r="I773" t="s">
+        <v>57</v>
+      </c>
+      <c r="J773" t="s">
+        <v>13</v>
+      </c>
+      <c r="K773" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="774" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A774" s="1">
+        <v>43335</v>
+      </c>
+      <c r="B774" t="s">
+        <v>89</v>
+      </c>
+      <c r="C774" t="s">
+        <v>76</v>
+      </c>
+      <c r="D774" t="s">
+        <v>60</v>
+      </c>
+      <c r="E774">
+        <v>1</v>
+      </c>
+      <c r="F774">
+        <v>5</v>
+      </c>
+      <c r="G774" t="s">
+        <v>26</v>
+      </c>
+      <c r="H774" t="s">
+        <v>45</v>
+      </c>
+      <c r="J774" t="s">
+        <v>13</v>
+      </c>
+      <c r="K774" s="1">
+        <v>43493</v>
+      </c>
+    </row>
+    <row r="775" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A775" s="1"/>
+      <c r="K775" s="1"/>
+    </row>
+    <row r="776" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A776" s="1"/>
+      <c r="K776" s="1"/>
+    </row>
+    <row r="777" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A777" s="1"/>
+      <c r="K777" s="1"/>
+    </row>
+    <row r="778" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A778" s="1"/>
+      <c r="K778" s="1"/>
+    </row>
+    <row r="779" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A779" s="1"/>
+      <c r="K779" s="1"/>
+    </row>
+    <row r="780" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A780" s="1"/>
+      <c r="K780" s="1"/>
+    </row>
+    <row r="781" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A781" s="1"/>
+      <c r="K781" s="1"/>
+    </row>
+    <row r="782" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A782" s="1"/>
+      <c r="K782" s="1"/>
+    </row>
+    <row r="783" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A783" s="1"/>
+      <c r="K783" s="1"/>
+    </row>
+    <row r="784" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A784" s="1"/>
+      <c r="K784" s="1"/>
+    </row>
+    <row r="785" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A785" s="1"/>
+      <c r="K785" s="1"/>
+    </row>
+    <row r="786" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A786" s="1"/>
+      <c r="K786" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bunch of fresh xls files for PC ORD
</commit_message>
<xml_diff>
--- a/Diets/Data/2018 Diets.xlsx
+++ b/Diets/Data/2018 Diets.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Master!$A$1:$L$685</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Master!$A$1:$L$786</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5049" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5049" uniqueCount="93">
   <si>
     <t>Coll. Date</t>
   </si>
@@ -297,9 +297,6 @@
     <t>Corydalidae</t>
   </si>
   <si>
-    <t>TAT</t>
-  </si>
-  <si>
     <t>W-113</t>
   </si>
   <si>
@@ -313,9 +310,6 @@
   </si>
   <si>
     <t>DIptera</t>
-  </si>
-  <si>
-    <t>Amph</t>
   </si>
 </sst>
 </file>
@@ -351,9 +345,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,8 +630,8 @@
   <dimension ref="A1:L786"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A767" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A775" sqref="A775:L797"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1410,7 +1406,7 @@
         <v>36</v>
       </c>
       <c r="J23" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="K23" s="1">
         <v>43410</v>
@@ -21993,7 +21989,7 @@
         <v>43333</v>
       </c>
       <c r="B635" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C635" t="s">
         <v>75</v>
@@ -22028,7 +22024,7 @@
         <v>43333</v>
       </c>
       <c r="B636" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C636" t="s">
         <v>75</v>
@@ -22063,7 +22059,7 @@
         <v>43333</v>
       </c>
       <c r="B637" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C637" t="s">
         <v>75</v>
@@ -22095,7 +22091,7 @@
         <v>43333</v>
       </c>
       <c r="B638" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C638" t="s">
         <v>75</v>
@@ -22127,7 +22123,7 @@
         <v>43333</v>
       </c>
       <c r="B639" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C639" t="s">
         <v>75</v>
@@ -22159,7 +22155,7 @@
         <v>43333</v>
       </c>
       <c r="B640" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C640" t="s">
         <v>75</v>
@@ -22191,7 +22187,7 @@
         <v>43333</v>
       </c>
       <c r="B641" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C641" t="s">
         <v>75</v>
@@ -22223,7 +22219,7 @@
         <v>43333</v>
       </c>
       <c r="B642" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C642" t="s">
         <v>75</v>
@@ -22255,7 +22251,7 @@
         <v>43333</v>
       </c>
       <c r="B643" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C643" t="s">
         <v>75</v>
@@ -22290,7 +22286,7 @@
         <v>43333</v>
       </c>
       <c r="B644" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C644" t="s">
         <v>75</v>
@@ -22322,7 +22318,7 @@
         <v>43333</v>
       </c>
       <c r="B645" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C645" t="s">
         <v>75</v>
@@ -22354,7 +22350,7 @@
         <v>43333</v>
       </c>
       <c r="B646" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C646" t="s">
         <v>75</v>
@@ -22386,7 +22382,7 @@
         <v>43333</v>
       </c>
       <c r="B647" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C647" t="s">
         <v>75</v>
@@ -22418,7 +22414,7 @@
         <v>43333</v>
       </c>
       <c r="B648" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C648" t="s">
         <v>75</v>
@@ -22450,7 +22446,7 @@
         <v>43333</v>
       </c>
       <c r="B649" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C649" t="s">
         <v>75</v>
@@ -22482,7 +22478,7 @@
         <v>43333</v>
       </c>
       <c r="B650" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C650" t="s">
         <v>75</v>
@@ -22514,7 +22510,7 @@
         <v>43333</v>
       </c>
       <c r="B651" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C651" t="s">
         <v>75</v>
@@ -22546,7 +22542,7 @@
         <v>43333</v>
       </c>
       <c r="B652" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C652" t="s">
         <v>75</v>
@@ -22581,7 +22577,7 @@
         <v>43333</v>
       </c>
       <c r="B653" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C653" t="s">
         <v>75</v>
@@ -22613,7 +22609,7 @@
         <v>43333</v>
       </c>
       <c r="B654" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C654" t="s">
         <v>75</v>
@@ -22645,7 +22641,7 @@
         <v>43333</v>
       </c>
       <c r="B655" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C655" t="s">
         <v>75</v>
@@ -22677,7 +22673,7 @@
         <v>43333</v>
       </c>
       <c r="B656" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C656" t="s">
         <v>75</v>
@@ -22709,7 +22705,7 @@
         <v>43333</v>
       </c>
       <c r="B657" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C657" t="s">
         <v>75</v>
@@ -22741,7 +22737,7 @@
         <v>43333</v>
       </c>
       <c r="B658" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C658" t="s">
         <v>75</v>
@@ -22773,7 +22769,7 @@
         <v>43333</v>
       </c>
       <c r="B659" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C659" t="s">
         <v>75</v>
@@ -22805,7 +22801,7 @@
         <v>43333</v>
       </c>
       <c r="B660" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C660" t="s">
         <v>75</v>
@@ -22837,7 +22833,7 @@
         <v>43333</v>
       </c>
       <c r="B661" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C661" t="s">
         <v>75</v>
@@ -22869,7 +22865,7 @@
         <v>43333</v>
       </c>
       <c r="B662" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C662" t="s">
         <v>75</v>
@@ -22901,7 +22897,7 @@
         <v>43333</v>
       </c>
       <c r="B663" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C663" t="s">
         <v>75</v>
@@ -22936,7 +22932,7 @@
         <v>43333</v>
       </c>
       <c r="B664" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C664" t="s">
         <v>75</v>
@@ -22971,7 +22967,7 @@
         <v>43333</v>
       </c>
       <c r="B665" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C665" t="s">
         <v>75</v>
@@ -23006,7 +23002,7 @@
         <v>43333</v>
       </c>
       <c r="B666" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C666" t="s">
         <v>75</v>
@@ -23041,7 +23037,7 @@
         <v>43333</v>
       </c>
       <c r="B667" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C667" t="s">
         <v>75</v>
@@ -23076,7 +23072,7 @@
         <v>43333</v>
       </c>
       <c r="B668" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C668" t="s">
         <v>75</v>
@@ -23108,7 +23104,7 @@
         <v>43333</v>
       </c>
       <c r="B669" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C669" t="s">
         <v>75</v>
@@ -23140,7 +23136,7 @@
         <v>43333</v>
       </c>
       <c r="B670" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C670" t="s">
         <v>75</v>
@@ -23175,7 +23171,7 @@
         <v>43333</v>
       </c>
       <c r="B671" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C671" t="s">
         <v>75</v>
@@ -23193,7 +23189,7 @@
         <v>26</v>
       </c>
       <c r="H671" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J671" t="s">
         <v>13</v>
@@ -23207,7 +23203,7 @@
         <v>43333</v>
       </c>
       <c r="B672" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C672" t="s">
         <v>75</v>
@@ -23242,7 +23238,7 @@
         <v>43333</v>
       </c>
       <c r="B673" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C673" t="s">
         <v>75</v>
@@ -23277,7 +23273,7 @@
         <v>43333</v>
       </c>
       <c r="B674" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C674" t="s">
         <v>75</v>
@@ -23312,7 +23308,7 @@
         <v>43333</v>
       </c>
       <c r="B675" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C675" t="s">
         <v>75</v>
@@ -23344,7 +23340,7 @@
         <v>43333</v>
       </c>
       <c r="B676" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C676" t="s">
         <v>75</v>
@@ -23376,7 +23372,7 @@
         <v>43333</v>
       </c>
       <c r="B677" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C677" t="s">
         <v>75</v>
@@ -23408,7 +23404,7 @@
         <v>43333</v>
       </c>
       <c r="B678" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C678" t="s">
         <v>75</v>
@@ -23440,7 +23436,7 @@
         <v>43333</v>
       </c>
       <c r="B679" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C679" t="s">
         <v>75</v>
@@ -23475,7 +23471,7 @@
         <v>43333</v>
       </c>
       <c r="B680" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C680" t="s">
         <v>75</v>
@@ -23507,7 +23503,7 @@
         <v>43333</v>
       </c>
       <c r="B681" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C681" t="s">
         <v>75</v>
@@ -23539,7 +23535,7 @@
         <v>43333</v>
       </c>
       <c r="B682" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C682" t="s">
         <v>75</v>
@@ -23571,7 +23567,7 @@
         <v>43333</v>
       </c>
       <c r="B683" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C683" t="s">
         <v>75</v>
@@ -23603,7 +23599,7 @@
         <v>43333</v>
       </c>
       <c r="B684" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C684" t="s">
         <v>75</v>
@@ -23638,7 +23634,7 @@
         <v>43333</v>
       </c>
       <c r="B685" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C685" t="s">
         <v>75</v>
@@ -23670,7 +23666,7 @@
         <v>43333</v>
       </c>
       <c r="B686" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C686" t="s">
         <v>75</v>
@@ -23702,7 +23698,7 @@
         <v>43333</v>
       </c>
       <c r="B687" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C687" t="s">
         <v>75</v>
@@ -23734,7 +23730,7 @@
         <v>43333</v>
       </c>
       <c r="B688" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C688" t="s">
         <v>75</v>
@@ -23766,7 +23762,7 @@
         <v>43333</v>
       </c>
       <c r="B689" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C689" t="s">
         <v>75</v>
@@ -23798,7 +23794,7 @@
         <v>43333</v>
       </c>
       <c r="B690" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C690" t="s">
         <v>75</v>
@@ -23819,7 +23815,7 @@
         <v>19</v>
       </c>
       <c r="I690" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J690" t="s">
         <v>17</v>
@@ -23833,7 +23829,7 @@
         <v>43333</v>
       </c>
       <c r="B691" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C691" t="s">
         <v>75</v>
@@ -23865,7 +23861,7 @@
         <v>43333</v>
       </c>
       <c r="B692" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C692" t="s">
         <v>75</v>
@@ -23897,7 +23893,7 @@
         <v>43333</v>
       </c>
       <c r="B693" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C693" t="s">
         <v>75</v>
@@ -23929,7 +23925,7 @@
         <v>43333</v>
       </c>
       <c r="B694" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C694" t="s">
         <v>75</v>
@@ -23961,7 +23957,7 @@
         <v>43333</v>
       </c>
       <c r="B695" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C695" t="s">
         <v>75</v>
@@ -23996,7 +23992,7 @@
         <v>43333</v>
       </c>
       <c r="B696" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C696" t="s">
         <v>75</v>
@@ -24028,7 +24024,7 @@
         <v>43333</v>
       </c>
       <c r="B697" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C697" t="s">
         <v>75</v>
@@ -24060,7 +24056,7 @@
         <v>43333</v>
       </c>
       <c r="B698" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C698" t="s">
         <v>75</v>
@@ -24092,7 +24088,7 @@
         <v>43333</v>
       </c>
       <c r="B699" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C699" t="s">
         <v>75</v>
@@ -24124,7 +24120,7 @@
         <v>43333</v>
       </c>
       <c r="B700" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C700" t="s">
         <v>75</v>
@@ -24156,7 +24152,7 @@
         <v>43333</v>
       </c>
       <c r="B701" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C701" t="s">
         <v>75</v>
@@ -24188,7 +24184,7 @@
         <v>43333</v>
       </c>
       <c r="B702" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C702" t="s">
         <v>75</v>
@@ -24220,7 +24216,7 @@
         <v>43333</v>
       </c>
       <c r="B703" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C703" t="s">
         <v>75</v>
@@ -24252,7 +24248,7 @@
         <v>43333</v>
       </c>
       <c r="B704" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C704" t="s">
         <v>75</v>
@@ -24284,7 +24280,7 @@
         <v>43333</v>
       </c>
       <c r="B705" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C705" t="s">
         <v>75</v>
@@ -24316,7 +24312,7 @@
         <v>43333</v>
       </c>
       <c r="B706" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C706" t="s">
         <v>75</v>
@@ -24348,7 +24344,7 @@
         <v>43333</v>
       </c>
       <c r="B707" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C707" t="s">
         <v>75</v>
@@ -24380,7 +24376,7 @@
         <v>43333</v>
       </c>
       <c r="B708" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C708" t="s">
         <v>75</v>
@@ -24412,7 +24408,7 @@
         <v>43333</v>
       </c>
       <c r="B709" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C709" t="s">
         <v>75</v>
@@ -24444,7 +24440,7 @@
         <v>43333</v>
       </c>
       <c r="B710" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C710" t="s">
         <v>75</v>
@@ -24476,7 +24472,7 @@
         <v>43333</v>
       </c>
       <c r="B711" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C711" t="s">
         <v>75</v>
@@ -24508,7 +24504,7 @@
         <v>43333</v>
       </c>
       <c r="B712" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C712" t="s">
         <v>75</v>
@@ -24540,7 +24536,7 @@
         <v>43333</v>
       </c>
       <c r="B713" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C713" t="s">
         <v>75</v>
@@ -24572,7 +24568,7 @@
         <v>43333</v>
       </c>
       <c r="B714" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C714" t="s">
         <v>75</v>
@@ -24607,7 +24603,7 @@
         <v>43335</v>
       </c>
       <c r="B715" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C715" t="s">
         <v>76</v>
@@ -24639,7 +24635,7 @@
         <v>43335</v>
       </c>
       <c r="B716" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C716" t="s">
         <v>76</v>
@@ -24671,7 +24667,7 @@
         <v>43335</v>
       </c>
       <c r="B717" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C717" t="s">
         <v>76</v>
@@ -24706,7 +24702,7 @@
         <v>43335</v>
       </c>
       <c r="B718" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C718" t="s">
         <v>76</v>
@@ -24738,7 +24734,7 @@
         <v>43335</v>
       </c>
       <c r="B719" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C719" t="s">
         <v>76</v>
@@ -24770,7 +24766,7 @@
         <v>43335</v>
       </c>
       <c r="B720" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C720" t="s">
         <v>76</v>
@@ -24805,7 +24801,7 @@
         <v>43335</v>
       </c>
       <c r="B721" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C721" t="s">
         <v>76</v>
@@ -24840,7 +24836,7 @@
         <v>43335</v>
       </c>
       <c r="B722" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C722" t="s">
         <v>76</v>
@@ -24872,7 +24868,7 @@
         <v>43335</v>
       </c>
       <c r="B723" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C723" t="s">
         <v>76</v>
@@ -24904,7 +24900,7 @@
         <v>43335</v>
       </c>
       <c r="B724" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C724" t="s">
         <v>76</v>
@@ -24936,7 +24932,7 @@
         <v>43335</v>
       </c>
       <c r="B725" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C725" t="s">
         <v>76</v>
@@ -24971,7 +24967,7 @@
         <v>43335</v>
       </c>
       <c r="B726" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C726" t="s">
         <v>76</v>
@@ -25006,7 +25002,7 @@
         <v>43335</v>
       </c>
       <c r="B727" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C727" t="s">
         <v>76</v>
@@ -25038,7 +25034,7 @@
         <v>43335</v>
       </c>
       <c r="B728" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C728" t="s">
         <v>76</v>
@@ -25070,7 +25066,7 @@
         <v>43335</v>
       </c>
       <c r="B729" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C729" t="s">
         <v>76</v>
@@ -25105,7 +25101,7 @@
         <v>43335</v>
       </c>
       <c r="B730" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C730" t="s">
         <v>76</v>
@@ -25140,7 +25136,7 @@
         <v>43335</v>
       </c>
       <c r="B731" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C731" t="s">
         <v>76</v>
@@ -25172,7 +25168,7 @@
         <v>43335</v>
       </c>
       <c r="B732" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C732" t="s">
         <v>76</v>
@@ -25207,7 +25203,7 @@
         <v>43335</v>
       </c>
       <c r="B733" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C733" t="s">
         <v>76</v>
@@ -25242,7 +25238,7 @@
         <v>43335</v>
       </c>
       <c r="B734" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C734" t="s">
         <v>76</v>
@@ -25277,7 +25273,7 @@
         <v>43335</v>
       </c>
       <c r="B735" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C735" t="s">
         <v>76</v>
@@ -25312,7 +25308,7 @@
         <v>43335</v>
       </c>
       <c r="B736" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C736" t="s">
         <v>76</v>
@@ -25347,7 +25343,7 @@
         <v>43335</v>
       </c>
       <c r="B737" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C737" t="s">
         <v>76</v>
@@ -25368,7 +25364,7 @@
         <v>19</v>
       </c>
       <c r="I737" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J737" t="s">
         <v>13</v>
@@ -25382,7 +25378,7 @@
         <v>43335</v>
       </c>
       <c r="B738" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C738" t="s">
         <v>76</v>
@@ -25400,10 +25396,10 @@
         <v>26</v>
       </c>
       <c r="H738" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I738" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J738" t="s">
         <v>13</v>
@@ -25417,7 +25413,7 @@
         <v>43335</v>
       </c>
       <c r="B739" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C739" t="s">
         <v>76</v>
@@ -25449,7 +25445,7 @@
         <v>43335</v>
       </c>
       <c r="B740" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C740" t="s">
         <v>76</v>
@@ -25481,7 +25477,7 @@
         <v>43335</v>
       </c>
       <c r="B741" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C741" t="s">
         <v>76</v>
@@ -25513,7 +25509,7 @@
         <v>43335</v>
       </c>
       <c r="B742" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C742" t="s">
         <v>76</v>
@@ -25545,7 +25541,7 @@
         <v>43335</v>
       </c>
       <c r="B743" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C743" t="s">
         <v>76</v>
@@ -25577,7 +25573,7 @@
         <v>43335</v>
       </c>
       <c r="B744" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C744" t="s">
         <v>76</v>
@@ -25609,7 +25605,7 @@
         <v>43335</v>
       </c>
       <c r="B745" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C745" t="s">
         <v>76</v>
@@ -25641,7 +25637,7 @@
         <v>43335</v>
       </c>
       <c r="B746" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C746" t="s">
         <v>76</v>
@@ -25673,7 +25669,7 @@
         <v>43335</v>
       </c>
       <c r="B747" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C747" t="s">
         <v>76</v>
@@ -25708,7 +25704,7 @@
         <v>43335</v>
       </c>
       <c r="B748" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C748" t="s">
         <v>76</v>
@@ -25743,7 +25739,7 @@
         <v>43335</v>
       </c>
       <c r="B749" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C749" t="s">
         <v>76</v>
@@ -25775,7 +25771,7 @@
         <v>43335</v>
       </c>
       <c r="B750" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C750" t="s">
         <v>76</v>
@@ -25810,7 +25806,7 @@
         <v>43335</v>
       </c>
       <c r="B751" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C751" t="s">
         <v>76</v>
@@ -25842,7 +25838,7 @@
         <v>43335</v>
       </c>
       <c r="B752" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C752" t="s">
         <v>76</v>
@@ -25872,38 +25868,38 @@
         <v>43493</v>
       </c>
     </row>
-    <row r="753" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A753" s="1">
+    <row r="753" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A753" s="2">
         <v>43335</v>
       </c>
-      <c r="B753" t="s">
-        <v>89</v>
-      </c>
-      <c r="C753" t="s">
-        <v>76</v>
-      </c>
-      <c r="D753" t="s">
-        <v>60</v>
-      </c>
-      <c r="E753">
-        <v>1</v>
-      </c>
-      <c r="F753">
+      <c r="B753" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C753" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D753" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E753" s="3">
+        <v>1</v>
+      </c>
+      <c r="F753" s="3">
         <v>4</v>
       </c>
-      <c r="G753" t="s">
-        <v>26</v>
-      </c>
-      <c r="H753" t="s">
+      <c r="G753" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H753" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I753" t="s">
-        <v>94</v>
-      </c>
-      <c r="J753" t="s">
+      <c r="I753" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J753" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K753" s="1">
+      <c r="K753" s="2">
         <v>43493</v>
       </c>
     </row>
@@ -25912,7 +25908,7 @@
         <v>43335</v>
       </c>
       <c r="B754" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C754" t="s">
         <v>76</v>
@@ -25947,7 +25943,7 @@
         <v>43335</v>
       </c>
       <c r="B755" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C755" t="s">
         <v>76</v>
@@ -25979,7 +25975,7 @@
         <v>43335</v>
       </c>
       <c r="B756" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C756" t="s">
         <v>76</v>
@@ -26014,7 +26010,7 @@
         <v>43335</v>
       </c>
       <c r="B757" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C757" t="s">
         <v>76</v>
@@ -26046,7 +26042,7 @@
         <v>43335</v>
       </c>
       <c r="B758" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C758" t="s">
         <v>76</v>
@@ -26078,7 +26074,7 @@
         <v>43335</v>
       </c>
       <c r="B759" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C759" t="s">
         <v>76</v>
@@ -26113,7 +26109,7 @@
         <v>43335</v>
       </c>
       <c r="B760" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C760" t="s">
         <v>76</v>
@@ -26145,7 +26141,7 @@
         <v>43335</v>
       </c>
       <c r="B761" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C761" t="s">
         <v>76</v>
@@ -26180,7 +26176,7 @@
         <v>43335</v>
       </c>
       <c r="B762" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C762" t="s">
         <v>76</v>
@@ -26212,7 +26208,7 @@
         <v>43335</v>
       </c>
       <c r="B763" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C763" t="s">
         <v>76</v>
@@ -26233,7 +26229,7 @@
         <v>19</v>
       </c>
       <c r="I763" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J763" t="s">
         <v>13</v>
@@ -26247,7 +26243,7 @@
         <v>43335</v>
       </c>
       <c r="B764" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C764" t="s">
         <v>76</v>
@@ -26282,7 +26278,7 @@
         <v>43335</v>
       </c>
       <c r="B765" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C765" t="s">
         <v>76</v>
@@ -26314,7 +26310,7 @@
         <v>43335</v>
       </c>
       <c r="B766" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C766" t="s">
         <v>76</v>
@@ -26346,7 +26342,7 @@
         <v>43335</v>
       </c>
       <c r="B767" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C767" t="s">
         <v>76</v>
@@ -26378,7 +26374,7 @@
         <v>43335</v>
       </c>
       <c r="B768" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C768" t="s">
         <v>76</v>
@@ -26410,7 +26406,7 @@
         <v>43335</v>
       </c>
       <c r="B769" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C769" t="s">
         <v>76</v>
@@ -26442,7 +26438,7 @@
         <v>43335</v>
       </c>
       <c r="B770" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C770" t="s">
         <v>76</v>
@@ -26477,7 +26473,7 @@
         <v>43335</v>
       </c>
       <c r="B771" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C771" t="s">
         <v>76</v>
@@ -26509,7 +26505,7 @@
         <v>43335</v>
       </c>
       <c r="B772" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C772" t="s">
         <v>76</v>
@@ -26541,7 +26537,7 @@
         <v>43335</v>
       </c>
       <c r="B773" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C773" t="s">
         <v>76</v>
@@ -26576,7 +26572,7 @@
         <v>43335</v>
       </c>
       <c r="B774" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C774" t="s">
         <v>76</v>
@@ -26652,6 +26648,7 @@
       <c r="K786" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L786"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>